<commit_message>
updates to preprocess module
</commit_message>
<xml_diff>
--- a/src/data/incose_guide_sections_df.xlsx
+++ b/src/data/incose_guide_sections_df.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d350839dcbf84db5/Desktop/github_projects/venv_aiswre/aiswre/src/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_08D160E1437B4E12A72D4C19F52F13EF797CFBCE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F24448A4-8AD5-46E0-9682-D6492A511AF2}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="264">
   <si>
     <t>start</t>
   </si>
@@ -41,12 +47,6 @@
   </si>
   <si>
     <t>examples</t>
-  </si>
-  <si>
-    <t>system_base_message</t>
-  </si>
-  <si>
-    <t>user_base_message</t>
   </si>
   <si>
     <t>system_message</t>
@@ -691,225 +691,304 @@
   </si>
   <si>
     <t>Requirement: {req}
-Criteria: {definition}
-Examples: {examples}</t>
+Criteria:
+ Need statements and requirement statements must conform to one of the agreed patterns, thus resulting in a well-structured complete statement. 
+Examples:
+ See Appendix C, for examples of need statements and requirement statement patterns. 4</t>
   </si>
   <si>
     <t>Requirement: {req}
-Criteria:  Need statements and requirement statements must conform to one of the agreed patterns, thus resulting in a well-structured complete statement. 
-Examples:  See Appendix C, for examples of need statements and requirement statement patterns. 4</t>
+Criteria:
+ Use the active voice in the need statement or requirement statement with the responsible entity clearly identified as the subject of the sentence. 
+Examples:
+ Unacceptable: The Identity of the Customer shall be confirmed. [This is unacceptable because it does not identify the entity that is responsible/accountable for confirming the identity.] Improved by adding the subject: The Identity of the Customer shall be confirmed by the Accounting_System. [Although this statement makes the subject clear, it is still unacceptable because the statement is in the passive voice in that the entity that is responsible/accountable for recording the audio is at the end of the statement rather than the beginning.] Improved: The Accounting_System shall confirm the Customer_Identity. Guide to Writing Requirements 66 [Note that “Accounting_System”, “confirm”, and “Customer_Identity” must be defined in the glossary since there are a number of possible interpretations of these terms—see R4. Also note that this statement is improved because it is in the active voice but, before it is acceptable, it needs to be further improved through the addition of appropriate condition and qualifying clauses] Unacceptable: While in the Operations_Mode, the Audio having the characteristics defined in &lt;ICD xxxx&gt; shall be recorded. [This is unacceptable because the entity that is responsible/accountable for recording the audio is not stated, which makes it difficult to identify which entity is responsible for the action, or how verification is to occur. In addition, the characteristics of the Audio are not referenced, nor are the conditions under which the action specified.] Improved by adding the subject: While in the Operations_Mode, the Audio having the characteristics defined in &lt;ICD xxxx&gt; shall be recorded by the &lt;SOI&gt;. [Although this statement makes the subject clear, it is still unacceptable because the statement is in the passive voice in that the entity that is responsible/accountable for recording the audio is at the end of the statement rather than the beginning.] Improved: While in the Operations_Mode, the &lt;SOI&gt; shall record Audio having the characteristics defined in &lt;ICD xxxx&gt;. [This is improved because it is in the active voice, but appropriate performance parameters should be added before the statement is acceptable. Also note that “Audio” must be defined in the glossary or data dictionary and required performance added for the requirement to be complete. The characteristics of the Audio received from a &lt;xxxx&gt; source is defined in the ICD.] 4</t>
   </si>
   <si>
     <t>Requirement: {req}
-Criteria:  Use the active voice in the need statement or requirement statement with the responsible entity clearly identified as the subject of the sentence. 
-Examples:  Unacceptable: The Identity of the Customer shall be confirmed. [This is unacceptable because it does not identify the entity that is responsible/accountable for confirming the identity.] Improved by adding the subject: The Identity of the Customer shall be confirmed by the Accounting_System. [Although this statement makes the subject clear, it is still unacceptable because the statement is in the passive voice in that the entity that is responsible/accountable for recording the audio is at the end of the statement rather than the beginning.] Improved: The Accounting_System shall confirm the Customer_Identity. Guide to Writing Requirements 66 [Note that “Accounting_System”, “confirm”, and “Customer_Identity” must be defined in the glossary since there are a number of possible interpretations of these terms—see R4. Also note that this statement is improved because it is in the active voice but, before it is acceptable, it needs to be further improved through the addition of appropriate condition and qualifying clauses] Unacceptable: While in the Operations_Mode, the Audio having the characteristics defined in &lt;ICD xxxx&gt; shall be recorded. [This is unacceptable because the entity that is responsible/accountable for recording the audio is not stated, which makes it difficult to identify which entity is responsible for the action, or how verification is to occur. In addition, the characteristics of the Audio are not referenced, nor are the conditions under which the action specified.] Improved by adding the subject: While in the Operations_Mode, the Audio having the characteristics defined in &lt;ICD xxxx&gt; shall be recorded by the &lt;SOI&gt;. [Although this statement makes the subject clear, it is still unacceptable because the statement is in the passive voice in that the entity that is responsible/accountable for recording the audio is at the end of the statement rather than the beginning.] Improved: While in the Operations_Mode, the &lt;SOI&gt; shall record Audio having the characteristics defined in &lt;ICD xxxx&gt;. [This is improved because it is in the active voice, but appropriate performance parameters should be added before the statement is acceptable. Also note that “Audio” must be defined in the glossary or data dictionary and required performance added for the requirement to be complete. The characteristics of the Audio received from a &lt;xxxx&gt; source is defined in the ICD.] 4</t>
+Criteria:
+ Ensure the subject and verb of the need or requirement statement are appropriate to the entity to which the statement refers. 
+Examples:
+ Subject examples: Business management requirements have the form “The &lt;business&gt; shall …”. For example, “ACME_Transport shall …”. Business operations requirements on business elements have the form “The &lt;business element&gt; shall …”. For example, requirements on personnel roles have the form: “The &lt;personnel role&gt; shall …”—such as, “The Production_Manager shall …”; “The Marketing_Manager shall …”. System level needs have the form “The &lt;stakeholders&gt; need the system to ……” System requirements have the form "The &lt;SOI&gt; shall ..."—for example, “The Aircraft shall …” Subsystem level needs have the form “The &lt;stakeholders&gt; need the &lt;subsystem&gt; to ……” Subsystem requirements have the form “The &lt;subsystem&gt; shall …" - for example, once the subsystems are defined: “The Engine shall …”; and “The Landing_Gear shall …”. Verb examples: System level stakeholder need: “The &lt;stakeholders&gt; need the &lt;SOI&gt; to process data received from &lt;other system&gt;.” System level requirement: “The &lt;SOI&gt; shall [process] data received from &lt;another system&gt;. having the characteristics defined in &lt;Interface Definition XYZ.&gt;” Through analysis, the verb/function “process” could be decomposed into sub functions such as “receive”, “store”, “calculate”, “report”, and “display”. Then a decision needs to be made regarding the specific subsystem or system element in which these sub functions are to be performed. If more than one subsystem or system element has a role in performing any one of the sub functions, that requirement should be communicated at the system level and allocated to the applicable subsystems or system elements. If a sub function is to be implemented by a single subsystem or system element, then the sub function requirement should be communicated at the subsystem or system element set of requirements and traced back to the higher-level requirement from which it was decomposed. Unacceptable system requirement: “The User shall ...” [As discussed in Section 1.8, this is unacceptable because the requirement should be on the system, not the user or operator of the system. This wording is often the result of writing requirements directly from user stories or resulting need statements, without doing the Guide to Writing Requirements 69 transformation of the use case or need into a requirement. Ask, what does the system have to do so that the need can be achieved?] Improved: “The &lt;SOI&gt; shall …”. Unacceptable: The &lt;SOI&gt; shall display the Current_Time on the &lt;Display Device&gt; per &lt;Display Standard xyz&gt;. [Again, “Current_Time” and “Display_Device” must be defined in the glossary or data dictionary. This statement is most likely unacceptable because the Display_Device is either a system element which is presumably at a level lower than the SOI (and is therefore not appropriate to this level), or the Display_Device is a system or system element outside the SOI (and therefore should be handled as an interface since requirements cannot be placed on it by this requirement set). The display standard would be developed by the organization that would define standards to be used when displaying all information by all applications the organization develops including fonts, font sizes, colors, spacing, brightness, human factors, etc.] Improved: The &lt;SOI&gt; shall display the Current_Time per &lt;Display Standard xyz&gt;. [This is improved because the action is appropriate to the level of the requirement set. Note that, before being an acceptable statement, appropriate condition and qualifying clauses must be added.] 4</t>
   </si>
   <si>
     <t>Requirement: {req}
-Criteria:  Ensure the subject and verb of the need or requirement statement are appropriate to the entity to which the statement refers. 
-Examples:  Subject examples: Business management requirements have the form “The &lt;business&gt; shall …”. For example, “ACME_Transport shall …”. Business operations requirements on business elements have the form “The &lt;business element&gt; shall …”. For example, requirements on personnel roles have the form: “The &lt;personnel role&gt; shall …”—such as, “The Production_Manager shall …”; “The Marketing_Manager shall …”. System level needs have the form “The &lt;stakeholders&gt; need the system to ……” System requirements have the form "The &lt;SOI&gt; shall ..."—for example, “The Aircraft shall …” Subsystem level needs have the form “The &lt;stakeholders&gt; need the &lt;subsystem&gt; to ……” Subsystem requirements have the form “The &lt;subsystem&gt; shall …" - for example, once the subsystems are defined: “The Engine shall …”; and “The Landing_Gear shall …”. Verb examples: System level stakeholder need: “The &lt;stakeholders&gt; need the &lt;SOI&gt; to process data received from &lt;other system&gt;.” System level requirement: “The &lt;SOI&gt; shall [process] data received from &lt;another system&gt;. having the characteristics defined in &lt;Interface Definition XYZ.&gt;” Through analysis, the verb/function “process” could be decomposed into sub functions such as “receive”, “store”, “calculate”, “report”, and “display”. Then a decision needs to be made regarding the specific subsystem or system element in which these sub functions are to be performed. If more than one subsystem or system element has a role in performing any one of the sub functions, that requirement should be communicated at the system level and allocated to the applicable subsystems or system elements. If a sub function is to be implemented by a single subsystem or system element, then the sub function requirement should be communicated at the subsystem or system element set of requirements and traced back to the higher-level requirement from which it was decomposed. Unacceptable system requirement: “The User shall ...” [As discussed in Section 1.8, this is unacceptable because the requirement should be on the system, not the user or operator of the system. This wording is often the result of writing requirements directly from user stories or resulting need statements, without doing the Guide to Writing Requirements 69 transformation of the use case or need into a requirement. Ask, what does the system have to do so that the need can be achieved?] Improved: “The &lt;SOI&gt; shall …”. Unacceptable: The &lt;SOI&gt; shall display the Current_Time on the &lt;Display Device&gt; per &lt;Display Standard xyz&gt;. [Again, “Current_Time” and “Display_Device” must be defined in the glossary or data dictionary. This statement is most likely unacceptable because the Display_Device is either a system element which is presumably at a level lower than the SOI (and is therefore not appropriate to this level), or the Display_Device is a system or system element outside the SOI (and therefore should be handled as an interface since requirements cannot be placed on it by this requirement set). The display standard would be developed by the organization that would define standards to be used when displaying all information by all applications the organization develops including fonts, font sizes, colors, spacing, brightness, human factors, etc.] Improved: The &lt;SOI&gt; shall display the Current_Time per &lt;Display Standard xyz&gt;. [This is improved because the action is appropriate to the level of the requirement set. Note that, before being an acceptable statement, appropriate condition and qualifying clauses must be added.] 4</t>
+Criteria:
+ Define all terms used within the need statement and requirement statement within an associated glossary and/or data dictionary. 
+Examples:
+ Unacceptable: The &lt;SOI&gt; shall display the current time as defined in &lt;Display Standard xyz&gt;. [This is unacceptable because it is ambiguous. What is “current”? In which time zone? To what degree of accuracy? In which format?] Improved: The &lt;SOI&gt; shall display the Current_Time as defined in &lt;Display Standard xyz&gt;. [Note that “Current_Time” must then be defined in the glossary or data dictionary in terms of accuracy, format, time zone, and units. Further, appropriate condition and qualifying clauses must be included before the statement is acceptable. In addition, the organization can define a display standard that applies to all products developed by the organizations concerning how information is to be displayed (fonts, colors, size, spacing, human factors, etc.] 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement: {req}
+Criteria:
+ Use the definite article “the” rather than the indefinite article “a”. 
+Examples:
+ Unacceptable: The &lt;SOI&gt; shall provide a time display. [This is unacceptable for a requirement because it is ambiguous—is the intent to provide a device to display the time or to display the time? If a device to display the time, then this is not appropriate to level. If to display a time - will any time displayed do? Is a one-off display of the time satisfactory? The writer's intention was most likely that they wanted the system to display continuously the current time in a format that is readable, yet if the developer provided a constant display of “10:00 am” (or even a one-off display of any time), they could argue (albeit unreasonably) that they have met the requirement; yet they would have clearly failed to meet the customer's need and intent. Note that, as a need statement: “The &lt;stakeholders&gt; need the &lt;SOI&gt; to display the time.”, the statement is arguably acceptable. However, as part of the transformation process, the requirement writers must remove the ambiguity - resulting in the following requirement statement (amongst others). Improved: The &lt;SOI&gt; shall display the Current_Time as defined in &lt;display standard xyz&gt;. [Note that “Current_Time” must be defined in the glossary or data dictionary since there are a number of possible meanings and formats of the more-general term “current time.” For completeness, condition and qualifying clauses must also be added before the requirement is acceptable. In addition, the organization can define a standard that applies to all products developed by the organizations concerning how information is to be displayed (fonts, colors, size, spacing, human factors, etc.] </t>
   </si>
   <si>
     <t>Requirement: {req}
-Criteria:  Define all terms used within the need statement and requirement statement within an associated glossary and/or data dictionary. 
-Examples:  Unacceptable: The &lt;SOI&gt; shall display the current time as defined in &lt;Display Standard xyz&gt;. [This is unacceptable because it is ambiguous. What is “current”? In which time zone? To what degree of accuracy? In which format?] Improved: The &lt;SOI&gt; shall display the Current_Time as defined in &lt;Display Standard xyz&gt;. [Note that “Current_Time” must then be defined in the glossary or data dictionary in terms of accuracy, format, time zone, and units. Further, appropriate condition and qualifying clauses must be included before the statement is acceptable. In addition, the organization can define a display standard that applies to all products developed by the organizations concerning how information is to be displayed (fonts, colors, size, spacing, human factors, etc.] 4</t>
+Criteria:
+ When stating quantities, all numbers should have appropriate and consistent units of measure explicitly stated using a common measurement system in terms of the thing the number refers. Guide to Writing Requirements 72 
+Examples:
+ Unacceptable: With power applied, The Circuit_Board shall &lt;…&gt; a temperature of less than 30 degrees. [This is unacceptable because the units used are stated without indicating the specific measurement system used.] Improved: With power applied, The Circuit_Board shall &lt;…&gt; a temperature of less than 30 degrees Celsius. Unacceptable: The &lt;SOI&gt; shall establish communications as defined in &lt;ICD xyz&gt; with at least 4 in less than or equal to 10 seconds. [This is unacceptable because the units used are incomplete. “4” of what?] Improved: The &lt;SOI&gt; shall &lt;establish communications&gt; as defined in &lt;ICD xyz&gt; with at least 4 satellites in less than or equal to 10 seconds Guide to Writing Requirements 73 [Note that the phrase “establish communications” is probably acceptable at the business level when used in a need statement, but the phrase would need further elaboration at lower levels so that the need is decomposed into verifiable requirements relating to frequency, type of communications (voice? data?), quality, bandwidth, etc. which would typically be defined in an ICD that defines the characteristics of the communication signal to be established.] Unacceptable: “The Fuel_System shall have a maximum fuel volume of 60 l”. “When the Fuel_System detects the Fuel_Tank volume is less than 500 ml, the Fuel_System shall notify the operator within 1 second.” [This is unacceptable because the two requirements use different units of measure (“l” and “ml”). Improved: “The Fuel_System shall have a maximum Fuel_Tank volume of 60 l “. “When the Fuel_System detects the Fuel_Tank volume is less than 0.5 l, the Fuel_System shall notify the operator within 1 second.” [Now both requirements are written using the same units of measure(liters).] Additional Acceptable: "The Fuel_System shall have a maximum Fuel_Tank volume of 60 l.” “When the Signal_System detects the Fuel_Tank volume is less than 50 ml, the Signal_System shall light the Low-Fuel_Iindicator within 1 second." [In this particular case, while the property (“Fuel_Tank volume”) remains the same, the component/element is different ("Fuel_System" vs "Signal_System"). The measurement unit can vary because we are dealing with different component–property pairs.] [Note that “Fuel_System” and “Fuel_Tank” must be defined in the glossary or data dictionary.] 4</t>
   </si>
   <si>
     <t xml:space="preserve">Requirement: {req}
-Criteria:  Use the definite article “the” rather than the indefinite article “a”. 
-Examples:  Unacceptable: The &lt;SOI&gt; shall provide a time display. [This is unacceptable for a requirement because it is ambiguous—is the intent to provide a device to display the time or to display the time? If a device to display the time, then this is not appropriate to level. If to display a time - will any time displayed do? Is a one-off display of the time satisfactory? The writer's intention was most likely that they wanted the system to display continuously the current time in a format that is readable, yet if the developer provided a constant display of “10:00 am” (or even a one-off display of any time), they could argue (albeit unreasonably) that they have met the requirement; yet they would have clearly failed to meet the customer's need and intent. Note that, as a need statement: “The &lt;stakeholders&gt; need the &lt;SOI&gt; to display the time.”, the statement is arguably acceptable. However, as part of the transformation process, the requirement writers must remove the ambiguity - resulting in the following requirement statement (amongst others). Improved: The &lt;SOI&gt; shall display the Current_Time as defined in &lt;display standard xyz&gt;. [Note that “Current_Time” must be defined in the glossary or data dictionary since there are a number of possible meanings and formats of the more-general term “current time.” For completeness, condition and qualifying clauses must also be added before the requirement is acceptable. In addition, the organization can define a standard that applies to all products developed by the organizations concerning how information is to be displayed (fonts, colors, size, spacing, human factors, etc.] </t>
+Criteria:
+ Avoid the use of vague terms. 
+Examples:
+ Unacceptable: The &lt;SOI&gt; shall usually be online. [This is unacceptable because “usually” is ambiguous - is availability what is meant?] Improved: The &lt;SOI&gt; shall have an Availability of greater than xx% over a period of greater than yyyy hours. [Note that “Availability” must be defined in the glossary or data dictionary since there are a number of possible ways of calculating that measure. Alternately, the availability could be expressed as a need. Then the organization responsible for transforming the need into a requirement could develop feasible concepts for meeting the needed availability and derived one or more well-formed requirements that result in the need being met.] Unacceptable: The Flight_Information_System shall display per &lt;Display Standard xyz&gt; the Tracking_Information for relevant aircraft within &lt;xxxx seconds&gt; of detection. [This is unacceptable because it does not make explicit which aircraft are relevant. Additionally, the statement allows the developer to decide what is relevant; such decisions are in the province of the customer, who should make the requirement explicit.] Improved: The Flight_Information_System shall display per &lt;Display Standard xyz&gt; the Tracking_Information of each Aircraft located less than or equal to 20 kilometers from the Airfield when in the Operations_Mode within &lt;xxxx seconds&gt; of detection. [Now it is clear for which aircraft the information needs to be displayed. Note that “Aircraft”, “Tracking_Information”, “Airfield”, and “Operations_Mode” must be defined in the glossary or data dictionary.] </t>
   </si>
   <si>
     <t>Requirement: {req}
-Criteria:  When stating quantities, all numbers should have appropriate and consistent units of measure explicitly stated using a common measurement system in terms of the thing the number refers. Guide to Writing Requirements 72 
-Examples:  Unacceptable: With power applied, The Circuit_Board shall &lt;…&gt; a temperature of less than 30 degrees. [This is unacceptable because the units used are stated without indicating the specific measurement system used.] Improved: With power applied, The Circuit_Board shall &lt;…&gt; a temperature of less than 30 degrees Celsius. Unacceptable: The &lt;SOI&gt; shall establish communications as defined in &lt;ICD xyz&gt; with at least 4 in less than or equal to 10 seconds. [This is unacceptable because the units used are incomplete. “4” of what?] Improved: The &lt;SOI&gt; shall &lt;establish communications&gt; as defined in &lt;ICD xyz&gt; with at least 4 satellites in less than or equal to 10 seconds Guide to Writing Requirements 73 [Note that the phrase “establish communications” is probably acceptable at the business level when used in a need statement, but the phrase would need further elaboration at lower levels so that the need is decomposed into verifiable requirements relating to frequency, type of communications (voice? data?), quality, bandwidth, etc. which would typically be defined in an ICD that defines the characteristics of the communication signal to be established.] Unacceptable: “The Fuel_System shall have a maximum fuel volume of 60 l”. “When the Fuel_System detects the Fuel_Tank volume is less than 500 ml, the Fuel_System shall notify the operator within 1 second.” [This is unacceptable because the two requirements use different units of measure (“l” and “ml”). Improved: “The Fuel_System shall have a maximum Fuel_Tank volume of 60 l “. “When the Fuel_System detects the Fuel_Tank volume is less than 0.5 l, the Fuel_System shall notify the operator within 1 second.” [Now both requirements are written using the same units of measure(liters).] Additional Acceptable: "The Fuel_System shall have a maximum Fuel_Tank volume of 60 l.” “When the Signal_System detects the Fuel_Tank volume is less than 50 ml, the Signal_System shall light the Low-Fuel_Iindicator within 1 second." [In this particular case, while the property (“Fuel_Tank volume”) remains the same, the component/element is different ("Fuel_System" vs "Signal_System"). The measurement unit can vary because we are dealing with different component–property pairs.] [Note that “Fuel_System” and “Fuel_Tank” must be defined in the glossary or data dictionary.] 4</t>
+Criteria:
+ Avoid the inclusion of escape clauses that state vague conditions or possibilities, such as “so far as is possible”, “as little as possible”, “where possible”, “as much as possible”, “if it should prove necessary”, “if necessary”, “to the extent necessary”, “as appropriate”, “as required”, “to the extent practical”, and “if practicable”. 
+Examples:
+ Unacceptable: The GPS shall, where there is sufficient space, display the User_Location in accordance with &lt;Display Standard xyz&gt;. [This is unacceptable because whether there is sufficient space is vague, ambiguous, and unverifiable. The requirement is clearer without the escape clause.] Improved: The GPS shall display the User_Location in accordance with &lt;Display Standard XYZ&gt;. [Note that appropriate performance measures must also be specified such as within what time, format, and accuracy. Also note that “GPS” and “User_Location” must be defined in the glossary or data dictionary.] 4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ Avoid open-ended, non-specific clauses such as “including but not limited to”, “etc.” and “and so on”. 
+Examples:
+ Unacceptable: The ATM shall display the Customer Account_Number, Account_Balance, and so on per &lt;Display Standard xyz&gt;. [This is unacceptable because it contains an opened list of what is to be displayed.] Guide to Writing Requirements 76 Improved: [Split into as many requirements as necessary to be complete. Note that the types of customer information to be displayed needs to be defined in the glossary.]: The ATM shall display the Customer Account_Number in accordance with &lt;Display Standard xyz&gt;. The ATM shall display the Customer Account_Balance in accordance with &lt;Display Standard xyz&gt;. The ATM shall display the Customer Account_Type in accordance with &lt;Display Standard xyz&gt;. The ATM shall display the Customer Account_Overdraft_Limit in accordance with &lt;Display Standard xyz&gt;. [Note: Some may feel that a bulleted list or table is acceptable. While, from a readability perspective, this may be true, from a requirement management perspective, each item in the bulleted list is still a requirement. Because of this requirement statements as in the example above should be written as individual statements especially when allocation, traceability, verification, and validation activities are specific to the single item. See also R17, R18, R22, and R28.] [Note the above examples are incomplete in that expected performance and under what conditions has not been included in the requirement statements.] 4.2 Concision 4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ Avoid the use of superfluous infinitives such as “to be designed to”, “to be able to”, “to be capable of”, “to enable”, “to allow”. 
+Examples:
+ Unacceptable: The Weapon_System shall be able to store the location of each Ordnance. [This is unacceptable because it contains the superfluous infinitive “be able to” which implies the requirement is ubiquitous in that it can be applied at any time, but it therefore begs the question as to the condition under which the feature can be invoked. However, this is acceptable for the stakeholder need: “The stakeholders need the Weapon_System to be able to store the location of each Ordnance.”] Improved: When &lt;condition&gt;he Weapon_System shall store the Location of each Ordnance. [This is better because the requirement applies only in a particular condition. Note that the terms “Weapon_System”, “Location”, and “Ordnance” must be defined in the glossary or data dictionary. To be complete the appropriate performance characteristics would also need to be defined and included within the requirement statement.] 4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ Use a separate clause for each condition or qualification. 
+Examples:
+ Unacceptable: The Navigation_Beacon shall provide Augmentation_Data having the characteristics defined in &lt;ICD xyz&gt; at an accuracy of less than or equal to 20 meters to each Maritime_User during Harbor_Harbor_Approach_Maneuvering (HHAM). [This is unacceptable because it inserts a phrase in such a way that the object of the sentence is separated from the verb.] Improved: The Navigation_Beacon shall provide Augmentation_Data having the characteristics defined in &lt;ICD xyz&gt; to each Maritime_User engaged in Harbor_Harbor_Approach_Maneuvering (HHAM), at an accuracy of less than or equal to 20 meters. [This rewrite places the basic function in an unbroken clause followed by the sub-clause describing performance. Note that: “Navigation_Beacon”, “Maritime_User”, and “Harbor_Harbor_Approach_Maneuvering (HHAM)” must be defined in the glossary or data dictionary. There is also an issue in that when discussing accuracy, precision needs to also be addressed.] 4.3 Non-ambiguity 4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ Use correct grammar. 
+Examples:
+ Unacceptable: The Weapon_System shall storing the location of all ordnance. [This is unacceptable because the grammatical error leads to uncertainty about the meaning.] Improved: The Weapon_System shall store the location of all Ordnance. [Note that “Ordnance” must be defined in the glossary to be explicit about the types of weapons and ammunition. Also, where the location is to be stored and the format of the data, must be addressed. The action “store” needs to be further evaluated to determine if that is an appropriate action (verb) for the Weapon_System vs a user interacting with the Weapon_System as discussed in R3. Additionally, to be complete any specific performance measures and conditions should be included within the requirement statement.] Unacceptable: When in the Active_State, the Record_Subsystem shall display each of the Names of the Line_Items, without obscuring the User_ID per &lt;Display Standard xyz&gt;. [This is unacceptable because the grammatical error involving the inappropriate placement of “each of”—it is most likely that a Line_Item has only one name.] Improved: When in the Active_State, the Record_Subsystem shall display on &lt;Display Device&gt; the Name of each Line_Item, without obscuring the User_ID per &lt;Display Standard XYZ.&gt;. [This is acceptable the ambiguity has been addressed. The requirement is now more complete in that it references where the information is to be display and the standard to be used concerning the display of the information. If there are any performance measures that apply, they would also need to be addressed.] Unacceptable: The &lt;corporate website&gt; shall only use Approved_Fonts. [This is unacceptable because it mandates that the website shall only use the designated fonts—that is, it is not expected to perform any other function except to use those fonts. This is clearly not what is meant but becomes ambiguous by the inappropriate grammar and the incorrect placement of the word “only”. What is most likely meant is that the only fonts to be used are the approved fonts defined in the organization’s display standard.] Improved: The &lt;corporate website&gt; shall display information using Approved_Fonts defined in &lt;Display Standard xyz&gt;. Guide to Writing Requirements 80 [This is better because the ambiguity has been addressed. To be acceptable, any conditions and qualifying clauses would also need to be added. If the organization has a standard for displaying information that addresses acceptable fonts, font sizes, colors, spacing, human factors, etc., the requirement should refer to that standard.] 4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ Use correct spelling. 
+Examples:
+ Unacceptable: The Weapon_System shall store the location of each ordinance. [This is unacceptable because the word “ordinance” means regulation or law. It is unlikely that the Weapon_System is interested in the location of ordinance (regulations). In the context of a Guide to Writing Requirements 81 weapon system, what the authors meant to use is "ordnance" as in weapons and ammunition, not “ordinance”.] Improved: The Weapon_System shall store the Location of each Ordnance. [Note that “Location” and “Ordnance” must be defined in the glossary or data dictionary to be explicit about the types of weapons and ammunition. The action “store” needs to be further evaluated to determine if that is an appropriate action (verb) for the Weapon_System vs a user interacting with the Weapon_System as discussed in R3. Additionally, to be complete any specific performance measures and conditions should be included within the requirement statement.] 4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ Use correct punctuation. 
+Examples:
+ Unacceptable: The Navigation_Beacon shall provide Augmentation_Data having the characteristics defined in &lt;ICD xyz&gt; to each Maritime_User, engaged in Harbor_Harbor_Approach_Maneuvering (HHA) at an accuracy of less than 20 meters. [This is unacceptable because the incorrectly placed comma in this sentence confuses the meaning, leading the reader to believe that the accuracy is related to the maneuver rather than to the augmentation data.] Improved: The Navigation_Beacon shall provide Navigation_Data having the characteristics defined in &lt;ICD xyz&gt; to each Maritime_User engaged in Harbor_Harbor_Approach_Maneuvering (HHA), at an accuracy of less than 20 meters. [The positioning of the comma now makes it clear that the accuracy and availability relate to the data. Also note that, while performance measures are included, the appropriate conditions are not addressed. Further “Navigation_Beacon”, “Navigation_Data”, “Maritime_User”, and “Harbor_Harbor_Approach_Maneuvering (HHA)” must be defined in the glossary or data dictionary.] Guide to Writing Requirements 82 4</t>
   </si>
   <si>
     <t xml:space="preserve">Requirement: {req}
-Criteria:  Avoid the use of vague terms. 
-Examples:  Unacceptable: The &lt;SOI&gt; shall usually be online. [This is unacceptable because “usually” is ambiguous - is availability what is meant?] Improved: The &lt;SOI&gt; shall have an Availability of greater than xx% over a period of greater than yyyy hours. [Note that “Availability” must be defined in the glossary or data dictionary since there are a number of possible ways of calculating that measure. Alternately, the availability could be expressed as a need. Then the organization responsible for transforming the need into a requirement could develop feasible concepts for meeting the needed availability and derived one or more well-formed requirements that result in the need being met.] Unacceptable: The Flight_Information_System shall display per &lt;Display Standard xyz&gt; the Tracking_Information for relevant aircraft within &lt;xxxx seconds&gt; of detection. [This is unacceptable because it does not make explicit which aircraft are relevant. Additionally, the statement allows the developer to decide what is relevant; such decisions are in the province of the customer, who should make the requirement explicit.] Improved: The Flight_Information_System shall display per &lt;Display Standard xyz&gt; the Tracking_Information of each Aircraft located less than or equal to 20 kilometers from the Airfield when in the Operations_Mode within &lt;xxxx seconds&gt; of detection. [Now it is clear for which aircraft the information needs to be displayed. Note that “Aircraft”, “Tracking_Information”, “Airfield”, and “Operations_Mode” must be defined in the glossary or data dictionary.] </t>
+Criteria:
+ Use a defined convention to express logical expressions such as “[X AND Y]”, “[X OR Y]”, [X XOR Y]”, “NOT [X OR Y]”. 
+Examples:
+ Unacceptable: The Engine_Management_System shall disengage the Speed_Control_Subsystem within &lt;TBD seconds&gt; when the Cruise_Control is engaged, and the Driver applies the Accelerator. [This is unacceptable because of the ambiguity of “and” could be confused with combining two separate thoughts. Instead use the form of a logical expression [X AND Y].] Improved: When [the Cruise_Control is Engaged] AND [the Accelerator is Applied], the Engine_Management_System shall Disengage the Speed_Control_Subsystem within &lt;TBD seconds&gt;. [“Engine_Management_System”, “Speed_Control_Subsystem”, “Disengage”, “Engaged”, “Accelerator”, “Applied”, and “Cruise_Control” must be defined in the glossary or data dictionary.] Guide to Writing Requirements 83 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement: {req}
+Criteria:
+ Avoid the use of the word “not”. 
+Examples:
+ Unacceptable: The &lt;SOI&gt; shall not fail. [This is unacceptable because verification of the requirement would require infinite time. The requirement is also infeasible in that, as written, the implication is to never fail, under any conditions.] Improved: The &lt;SOI&gt; shall have an Availability of greater than or equal to 95%. or The &lt;SOI&gt; shall have a Mean Time Between Failures (MTBF) of xx operating hours. [For quality requirements, it would be more precise in the above were written as need statements. Then those transforming the quality need statements into requirement statements would define feasible concepts that would result in the needed quality attributes and derive well- formed requirements on the &lt;SOI&gt; that would result in those needs to be met.] Unacceptable: The &lt;SOI&gt; shall not contain mercury. [This is unacceptable because verification of the requirement would require the ability to measure the amount of mercury with infinite accuracy and precision. In addition, the real requirement may not be stated, for example, the real concern may be the use of toxic materials, not just mercury. If that is the case, it may be best to reference a standard from a governmental agency concerning allowable exposures to a list of common toxic materials.] Improved: The &lt;SOI&gt; shall limit metallic mercury exposure to those coming in contact with the &lt;SOI&gt; to less than or equal 0.025 mg/m3 over a period of 8 hours. </t>
   </si>
   <si>
     <t>Requirement: {req}
-Criteria:  Avoid the inclusion of escape clauses that state vague conditions or possibilities, such as “so far as is possible”, “as little as possible”, “where possible”, “as much as possible”, “if it should prove necessary”, “if necessary”, “to the extent necessary”, “as appropriate”, “as required”, “to the extent practical”, and “if practicable”. 
-Examples:  Unacceptable: The GPS shall, where there is sufficient space, display the User_Location in accordance with &lt;Display Standard xyz&gt;. [This is unacceptable because whether there is sufficient space is vague, ambiguous, and unverifiable. The requirement is clearer without the escape clause.] Improved: The GPS shall display the User_Location in accordance with &lt;Display Standard XYZ&gt;. [Note that appropriate performance measures must also be specified such as within what time, format, and accuracy. Also note that “GPS” and “User_Location” must be defined in the glossary or data dictionary.] 4</t>
+Criteria:
+ Avoid the use of the oblique (“/”) symbol. 
+Examples:
+ Unacceptable: The User_Management_System shall Open/Close the User_Account in less than 1 second. [This is unacceptable because it is unclear as to what is meant by open/close: open, close, or both?] Improved: (Split into two requirements with an appropriate condition) When &lt;condition&gt;, the User_Management_System shall Open the User_Account in less than 1 second. When &lt;condition&gt;, the User_Management_System shall Close the User_Account in less than 1 second. Unacceptable: When the Clutch is Disengaged and/or the Brake is Applied, the Engine_Management_System shall disengage the Speed_Control_Subsystem within &lt;XYZ ms&gt;. [This is unacceptable because of the use of “and/or.” If simultaneity is intended—that is the dual conditions must be met at the same time—write the requirements as a logical AND. If “and” is meant in the sense that the action is to be completed under each of the conditions, split the two thoughts into separate requirements, one for each condition. If “or” is meant, write the requirement as a logical OR.] Improved: (As one requirement if simultaneity is intended): When [the Clutch is Disengaged] AND [the Brake is Applied], the Engine_Management_System shall disengage the Speed_Control_Subsystem within &lt;XYZ ms&gt;. Guide to Writing Requirements 85 Improved: (As two requirements if two separate conditions are intended): When the Clutch is Disengaged, the Engine_Management_System shall disengage the Speed_Control_Subsystem within &lt;XYZ ms&gt;. When the Brake is Applied, the Engine_Management_System shall disengage the Speed_Control_Subsystem within &lt;XYZ ms&gt;. Improved: (As one requirement if inclusive OR is intended) When EITHER [the Clutch is Disengaged] OR [the Brake is Applied], the Engine_Management_System shall disengage the Speed_Control_Subsystem. 4.4 Singularity 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement: {req}
+Criteria:
+ Write a single sentence that contains a single thought conditioned and qualified by relevant sub- clauses. 
+Examples:
+ Unacceptable: When in the Active_State, the Record_Subsystem shall display the Name of each Line_Item and shall record the Location of each Line_Item, without obscuring the User_ID. [This is unacceptable because the sentence contains two requirements and the qualification only applies to the first requirement, not the second.] Improved: (Split into two separate requirements) When in the Active_State, the Record_Subsystem shall display per &lt;Display Standard XYZ&gt; the Name of each Line_Item, without obscuring the User_ID. When in the Active_ State, the Record_Subsystem shall record the Location of each Line_Item. [Note use of the glossary or data dictionary to define terms. Any applicable performance measures must be addressed for the requirement to be complete.] Unacceptable: The Control_Subsystem will close the Inlet_Valve until the temperature has reduced to 85 °C, when it will then reopen it in less than 1 second. [This is unacceptable because the sentence contains two event driven requirements. Additionally, the sentence contains two occurrences of the pronoun “it” ambiguously referring to different things (see R26), the term “has reduced” is ambiguous, and the action verb must be ”shall”, not “will”. Also, a time constraint is included but it is not clear whether it applies to both actions or only the second action.] Improved: (Split into two requirements each with its own time constraint): If the Water_Temperature in the Boiler increases to greater than 85 °C, the Control_Subsystem shall close the Inlet_Valve in less than 1 second. When the Water_Temperature in the Boiler reduces to less than or equal to 85 °C, the Control_Subsystem shall open the Inlet_Valve in less than 1 second. [Note use of the glossary or data dictionary to define terms.] Unacceptable: In the event of a fire detection, within &lt;xxx ms&gt;: • Security entrances shall be set to Free_Access_Mode. • Fire escape doors shall be unlocked. [This is unacceptable because the condition “in the event of a fire detection” is stated following a list of actions to be taken; each of which the system must be verified against. Also, note the actions are written in passive voice which violates R2. Each action needs to be communicated in a separate active voice requirement statement. For multiple conditions for a single action see R28.] Improved: (Split into two requirements) In the event of Fire_Detection, the Fire_Control_Subsystem shall set the Free_Access_Mode to ON within &lt;xxx ms&gt;. In the event of Fire_Detection, the Fire_Control_Subsystem shall send the Fire_Door_Unlock unlock command having the characteristics defined in &lt;ICD xyz&gt; to each Fire_Door within &lt;xxx ms&gt;. [There is a Fire Detection subsystem responsible for detecting fires and setting the Fire_Detection parameter to “TRUE” which triggers the two actions. All other subsystems that Guide to Writing Requirements 87 are monitoring when the Fire_Control_Subsystem has set the Free_Access_Mode to “TRUE” will take the required action as stated in their set of requirements. All Fire Doors will be monitoring for the Fire_Door_Unlock command and will unlock when the command is received.] Unacceptable: The &lt;corporate website&gt; shall use only approved fonts. The approved fonts are: &lt;Font1&gt;, &lt;Font2&gt; and &lt;Font3&gt;. [This is unacceptable because it is non-singular. Rather than splitting into three requirements (which is quite difficult to so whilst conforming to the “only” constraint, the term “Approved_Fonts” can be included in the Glossary, which then states: “Approved_Fonts: &lt;Font1&gt;, &lt;Font2&gt; and &lt;Font3&gt;.”] Improved: (using the glossary term “Approved_Fonts”) The &lt;corporate website&gt; shall use only Approved_Fonts. [Alternately, the organization can define a display standard which includes a definition of approved fonts, and the requirement could reference that standard.] Improved: (referring to a standard.) The &lt;corporate website&gt; shall display information in accordance with &lt;Display Standard xyz&gt;. [Note that this also allows better configuration management of the requirements database, particularly if the approved fonts are referred to in a number of requirements—that is, should the approved fonts change or characteristics of the fonts change, the list of approved fonts and characteristics only needs to be updated in the Glossary, rather than in multiple requirements (in which case there is a risk that one or more of the requirements is missed).] [In reality, requirements involving the actions such as “display” are interface requirements given that the information will be provided by something to some display device for display.] [Having the information in the display standard then can be referred to in the set of requirements for that display device. Note that referring to a standard also allows for later specialization, for example different parts of the standard may apply to different display devices.] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement: {req}
+Criteria:
+ Avoid words that join or combine clauses, such as “and”, “or”, “then”, “unless”, “but”, “as well as” “but also”, “however”, “whether”, “meanwhile”, “whereas”, “on the other hand”, or “otherwise”. 
+Examples:
+ Unacceptable: The user shall either be trusted or not trusted. [This is unacceptable for several reasons. The intention is that a user should be classified in one of two ways, but it is also a passive requirement written on the user rather than on the system (R2) and it is ambiguous: the requirement would still be met if the system took the option of treating all users as trusted.] Improved: The Security_System shall categorize each User as EITHER Trusted OR Not_Trusted. Unacceptable: The &lt;SOI&gt; shall display the Location and Identity of the Lead_Vehicle. [This is unacceptable because is in fact stating two requirements which may well need to be verified by different verification actions. In addition, the format of the displayed information is not referenced.] Improved: (Express as two requirements) The &lt;SOI&gt; shall display the Location of the Lead_Vehicle per &lt;Display Standard xyx&gt;. The &lt;SOI&gt; shall display the Identity of the Lead_Vehicle per &lt;Display Standard xyx&gt;. Unacceptable: The &lt;SOI&gt; shall provide an audible or visual alarm having the characteristics defined in &lt;alarm standard xyz&gt;. [This is unacceptable because it is a moot point as to whether the designer can choose which alarm to implement, or (which is probably the intent of the writer) whether both alarms are required, and the operator is alerted by at least one.] Improved: (if the choice is available to the designer) The &lt;SOI&gt; shall provide EITHER an Audible_Alarm OR Visual_Alarm having the characteristics defined in &lt;Alarm Standard xyz&gt;. Improved: (if both alarms are required) Guide to Writing Requirements 89 The &lt;SOI&gt; shall provide an Audible_Alarm having the characteristics defined in &lt;Alarm Standard xyz&gt;. The &lt;SOI&gt; shall provide a Visual_Alarm having the characteristics defined in &lt;Alarm Standard xyz&gt;. [As separate requirements, each can be allocated differently, and the SOI will be verified to meet each. </t>
   </si>
   <si>
     <t>Requirement: {req}
-Criteria:  Avoid open-ended, non-specific clauses such as “including but not limited to”, “etc.” and “and so on”. 
-Examples:  Unacceptable: The ATM shall display the Customer Account_Number, Account_Balance, and so on per &lt;Display Standard xyz&gt;. [This is unacceptable because it contains an opened list of what is to be displayed.] Guide to Writing Requirements 76 Improved: [Split into as many requirements as necessary to be complete. Note that the types of customer information to be displayed needs to be defined in the glossary.]: The ATM shall display the Customer Account_Number in accordance with &lt;Display Standard xyz&gt;. The ATM shall display the Customer Account_Balance in accordance with &lt;Display Standard xyz&gt;. The ATM shall display the Customer Account_Type in accordance with &lt;Display Standard xyz&gt;. The ATM shall display the Customer Account_Overdraft_Limit in accordance with &lt;Display Standard xyz&gt;. [Note: Some may feel that a bulleted list or table is acceptable. While, from a readability perspective, this may be true, from a requirement management perspective, each item in the bulleted list is still a requirement. Because of this requirement statements as in the example above should be written as individual statements especially when allocation, traceability, verification, and validation activities are specific to the single item. See also R17, R18, R22, and R28.] [Note the above examples are incomplete in that expected performance and under what conditions has not been included in the requirement statements.] 4.2 Concision 4</t>
+Criteria:
+ Avoid phrases that indicate the “purpose of “, “intent of”, or “reason for” the need statement or requirement statement. 
+Examples:
+ Unacceptable: The Record_Subsystem shall display the Name of each Line_Item so that the Operator can confirm that it is the correct Item. [This is unacceptable because the text “so that the Operator can confirm that it is the correct Item” is rationale.] Improved: The Record_Subsystem shall display the Name of each Line_Item per &lt;Display Standard XYZ&gt;. [The text “so that the Operator can confirm that it is the correct Item” should be included in the rationale attribute.] Guide to Writing Requirements 90 Unacceptable: The Operation_Logger shall record each Warning_Message produced by the system. [This is unacceptable because of the superfluous words “produced by the system”.] Improved: The Operation_Logger shall record each Warning_Message within &lt;performance measure&gt;. 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement: {req}
+Criteria:
+ Avoid parentheses and brackets containing subordinate text. 
+Examples:
+ Unacceptable: When the Water_Temperature exceeds 85 °C (usually towards the end of the boiling cycle), the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt; [This is unacceptable because of the parenthetical phrase as well as the ambiguous word “usually”. Note that the parameter Water_Temperature needs to be defined in the glossary in order to be specific] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt;. [Note: for the above example, if this behavior is the result of a design decision, then the requirement needs to be communicated as a design output. The design input requirement should focus on why this behavior is needed - for example, prevent the boiler from over pressurizing and exploding. This is a good example of the benefit of asking “Why” for requirements of this type. The answer is the real design input requirement. If included in the set of Design Input Requirements, then the “why” should be included in the rationale.] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall prevent the Boiler from over pressurization. [How this is done is a design decision.} </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement: {req}
+Criteria:
+ Enumerate sets explicitly instead of using a group noun to name the set. 
+Examples:
+ Unacceptable: The thermal control system shall manage temperature-related functions. [This is unacceptable because there is ambiguity regarding which functions are to be managed as well as what is meant by “managed”. The specific functions should be enumerated explicitly in separate requirement statements along with performance expectations and any applicable conditions, triggers, or constraints.] Unacceptable: The thermal control system shall monitor system temperature. This is unacceptable because there is ambiguity regarding the function “monitor”. Similar to “managed” What are the expectations of the stakeholders – update the display of the system temperature, maintain the temperature within some range, or store the history of the system temperature? The specific subfunctions should be enumerated explicitly in separate requirement statements along with performance expectations and any applicable conditions, triggers, or constraints.] Improved: (three separate requirements): The Thermal_Control_System shall update the display of System_Temperature every 10 +/- 1 seconds. The Thermal_Control_System shall maintain the System_Temperature between 95°C and 98°C. The Thermal_Control_System shall store the history of System_Temperature. [Note use of the glossary to define terms.] </t>
   </si>
   <si>
     <t>Requirement: {req}
-Criteria:  Avoid the use of superfluous infinitives such as “to be designed to”, “to be able to”, “to be capable of”, “to enable”, “to allow”. 
-Examples:  Unacceptable: The Weapon_System shall be able to store the location of each Ordnance. [This is unacceptable because it contains the superfluous infinitive “be able to” which implies the requirement is ubiquitous in that it can be applied at any time, but it therefore begs the question as to the condition under which the feature can be invoked. However, this is acceptable for the stakeholder need: “The stakeholders need the Weapon_System to be able to store the location of each Ordnance.”] Improved: When &lt;condition&gt;he Weapon_System shall store the Location of each Ordnance. [This is better because the requirement applies only in a particular condition. Note that the terms “Weapon_System”, “Location”, and “Ordnance” must be defined in the glossary or data dictionary. To be complete the appropriate performance characteristics would also need to be defined and included within the requirement statement.] 4</t>
+Criteria:
+ When a need or requirement is related to complex behavior, refer to a supporting diagram, model, or ICD. 
+Examples:
+ Unacceptable: The Control_System shall close Valves A AND B within 5 seconds of the temperature exceeding 95 °C AND within 2 seconds of each other. [This is unacceptable because of the confusing set of conditions. In this case what is meant will be clear if the requirement referred to a diagram for context.] Improved: [Within 5 seconds of the temperature exceeding 95 °C] AND [within 2 seconds of each other as shown in Timing_Diagram_6], the Control_System shall close [Valve A AND Valve B]. [Note that this assumes, of course, that the timing diagram itself is not ambiguous. If it is not possible to remove the ambiguity by using a diagram, it may be better to split the requirement into two.] [Note: for the above example, if this complex behavior is the result of a design decision, then the requirement needs to be communicated as a design output. The design input requirement should focus on why this behavior is needed.] Interface Example: An interface requirement may refer to the characteristics of the electrical power (current/voltage) being supplied by a system. There can be multiple characteristics that need to be defined such that the systems receiving the power have a clear understanding of the characteristics of the power they are receiving. In this case it is common for the characteristics to be defined in an ICD which both the provider and receiver of the power can refer to in their Design Input Requirements. From the provider perspective the provider system will have to be verified that the power provided has all of these characteristics and the receiver will have to verify it can receive and operate on power having these same characteristics. &lt;System 1&gt; shall provide power to &lt;System 2&gt; having the characteristics defined in &lt;ICD xyz&gt;. Table 123&gt;. &lt;System 2&gt; shall receive power from &lt;System 1&gt; having the characteristics defined in &lt;ICD xyz&gt;. Table 123&gt;. &lt;System 2&gt; shall operate on power having the characteristics defined in &lt;ICD xyz&gt;. Table 123&gt;. 4.5 Completeness 4</t>
   </si>
   <si>
     <t>Requirement: {req}
-Criteria:  Use a separate clause for each condition or qualification. 
-Examples:  Unacceptable: The Navigation_Beacon shall provide Augmentation_Data having the characteristics defined in &lt;ICD xyz&gt; at an accuracy of less than or equal to 20 meters to each Maritime_User during Harbor_Harbor_Approach_Maneuvering (HHAM). [This is unacceptable because it inserts a phrase in such a way that the object of the sentence is separated from the verb.] Improved: The Navigation_Beacon shall provide Augmentation_Data having the characteristics defined in &lt;ICD xyz&gt; to each Maritime_User engaged in Harbor_Harbor_Approach_Maneuvering (HHAM), at an accuracy of less than or equal to 20 meters. [This rewrite places the basic function in an unbroken clause followed by the sub-clause describing performance. Note that: “Navigation_Beacon”, “Maritime_User”, and “Harbor_Harbor_Approach_Maneuvering (HHAM)” must be defined in the glossary or data dictionary. There is also an issue in that when discussing accuracy, precision needs to also be addressed.] 4.3 Non-ambiguity 4</t>
+Criteria:
+ Avoid the use of personal and indefinite pronouns. 
+Examples:
+ Unacceptable: The controller shall send the driver his itinerary for the day. It shall be delivered at least 8 hours prior to his Shift. [This is unacceptable because the requirement is expressed as two sentences and the second sentence uses the pronouns “it” and “his.”] Improved: At least 8 hours prior to the Driver_Shift, the Controller shall send the Driver_Itinerary for the day to the Driver. [Note use of the glossary to define terms and to be explicit about the relationship between the driver, shift, and the itinerary for that particular driver.] 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement: {req}
+Criteria:
+ Avoid relying on headings to support explanation or understanding of the need or requirement. 
+Examples:
+ Example heading: “4.0 Alert Buzzer Requirements.” Unacceptable: 4.1 The &lt;SOI&gt; shall sound it for greater than 20 minutes. [This is unacceptable because the requirement uses the pronoun “it” (R24), which requires the heading to understand what “it” means. In addition, the word “sound” could be ambiguous as it can be a noun, a verb, adverb, or adjective. We do not know whether Alert_Buzzer is a subsystem that controls the noise or the thing that makes the noise.] Improved: When &lt;triggering event&gt;, the &lt;SOI&gt; shall sound an alert having the characteristics defined in &lt;Alert Standard xyz&gt; for greater than 20 minutes. [In this improved rewrite, the existence of the header is not needed to interpret the requirement. Even though the above heading referenced an “Alert Buzzer”—an implementation, the improved requirement avoids implementation to a specific device, and rather indicates that when the triggering event happens, an alert is required to be sounded having the characteristics defined in the alert standard. </t>
   </si>
   <si>
     <t>Requirement: {req}
-Criteria:  Use correct grammar. 
-Examples:  Unacceptable: The Weapon_System shall storing the location of all ordnance. [This is unacceptable because the grammatical error leads to uncertainty about the meaning.] Improved: The Weapon_System shall store the location of all Ordnance. [Note that “Ordnance” must be defined in the glossary to be explicit about the types of weapons and ammunition. Also, where the location is to be stored and the format of the data, must be addressed. The action “store” needs to be further evaluated to determine if that is an appropriate action (verb) for the Weapon_System vs a user interacting with the Weapon_System as discussed in R3. Additionally, to be complete any specific performance measures and conditions should be included within the requirement statement.] Unacceptable: When in the Active_State, the Record_Subsystem shall display each of the Names of the Line_Items, without obscuring the User_ID per &lt;Display Standard xyz&gt;. [This is unacceptable because the grammatical error involving the inappropriate placement of “each of”—it is most likely that a Line_Item has only one name.] Improved: When in the Active_State, the Record_Subsystem shall display on &lt;Display Device&gt; the Name of each Line_Item, without obscuring the User_ID per &lt;Display Standard XYZ.&gt;. [This is acceptable the ambiguity has been addressed. The requirement is now more complete in that it references where the information is to be display and the standard to be used concerning the display of the information. If there are any performance measures that apply, they would also need to be addressed.] Unacceptable: The &lt;corporate website&gt; shall only use Approved_Fonts. [This is unacceptable because it mandates that the website shall only use the designated fonts—that is, it is not expected to perform any other function except to use those fonts. This is clearly not what is meant but becomes ambiguous by the inappropriate grammar and the incorrect placement of the word “only”. What is most likely meant is that the only fonts to be used are the approved fonts defined in the organization’s display standard.] Improved: The &lt;corporate website&gt; shall display information using Approved_Fonts defined in &lt;Display Standard xyz&gt;. Guide to Writing Requirements 80 [This is better because the ambiguity has been addressed. To be acceptable, any conditions and qualifying clauses would also need to be added. If the organization has a standard for displaying information that addresses acceptable fonts, font sizes, colors, spacing, human factors, etc., the requirement should refer to that standard.] 4</t>
+Criteria:
+ Avoid using unachievable absolutes. 
+Examples:
+ Unacceptable: The &lt;SOI&gt; shall have 100% availability. [This is unacceptable because 100% is an absolute that is impossible to achieve and verify. Also, available over what time period?] Improved: The &lt;SOI&gt; shall have an Availability of greater than or equal to 98% during Operating_Hours. [Note use of the glossary to define Operating_Hours. Alternatively, this requirement could be stated as a need. Then those transforming the need into requirements would develop a Guide to Writing Requirements 96 feasible concept for doing so and then derive specific Design Input Requirements that would result in the need being met.] Unacceptable: The Pumping_Station shall maintain the flow of water at 100 liters per second for 30 minutes. [This is unacceptable because the requirement is impossibly precise to maintain in terms of the flow rate (and impossibly precise to measure in verification) as well as being impossibly precise to deliver for 30 minutes exactly. Also, it is not clear under what conditions this applies—when in operations, when powered on, when commanded?] Improved: When in operations, the Pumping_Station shall maintain Water_Flow at 100 ±10 liters per second for greater than 30 minutes. [Now the range of acceptable flow performance and time frame is clear and feasible. Given that the condition “when in operations” this requirement applies whenever the Pumping_Station is active—no matter how long. Also, what is the intent for how long—31 minutes satisfies the requirement, but what if the real intent is for however long the Pumping Station is in operations which could be hours or days—again depending on the operating conditions and need. Further, is the 30 minutes of continuous flow or a total of 30 minutes within a set time period?] 4.7 Conditions 4</t>
   </si>
   <si>
     <t>Requirement: {req}
-Criteria:  Use correct spelling. 
-Examples:  Unacceptable: The Weapon_System shall store the location of each ordinance. [This is unacceptable because the word “ordinance” means regulation or law. It is unlikely that the Weapon_System is interested in the location of ordinance (regulations). In the context of a Guide to Writing Requirements 81 weapon system, what the authors meant to use is "ordnance" as in weapons and ammunition, not “ordinance”.] Improved: The Weapon_System shall store the Location of each Ordnance. [Note that “Location” and “Ordnance” must be defined in the glossary or data dictionary to be explicit about the types of weapons and ammunition. The action “store” needs to be further evaluated to determine if that is an appropriate action (verb) for the Weapon_System vs a user interacting with the Weapon_System as discussed in R3. Additionally, to be complete any specific performance measures and conditions should be included within the requirement statement.] 4</t>
+Criteria:
+ State conditions’ applicability explicitly instead of leaving applicability to be inferred from the context. 
+Examples:
+ Unacceptable: The Free_Access_Mode shall be set to ON within &lt;xxx ms&gt;. The Fire_Door_Unlock command having the characteristics defined in &lt;ICD xyz&gt; shall be sent to each Fire_Door within &lt;xxx ms&gt;. [This is unacceptable because the condition or trigger for these actions is not stated. Also, note the actions are written in passive voice which violates R2. Each action needs to be communicated in a separate active voice requirement statement with the condition or trigger for which the action is to be initiated. For multiple conditions for a single action see R28.] Improved: (Split into two requirements) In the event of Fire_Detection, the Fire_Control_Subsystem shall set the Free_Access_Mode to ON within &lt;xxx ms&gt;. In the event of Fire_Detection, the Fire_Control_Subsystem shall send the Fire_Door_Unlock unlock command having the characteristics defined in &lt;ICD xyz&gt; to each Fire_Door within &lt;xxx ms&gt;. [Note that there is a Fire Detection subsystem responsible for detecting fires and setting the Fire_Detection parameter to “TRUE” which triggers the two actions. All other subsystems that are monitoring when the Fire_Control_Subsystem has set the Free_Access_Mode to “TRUE” will have their own requirements to monitor this parameter and take the required action(s) as stated in their set of requirements. All Fire Doors will have their own requirements to monitor for the Fire_Door_Unlock command and to unlock when the command is received.] 4</t>
   </si>
   <si>
     <t>Requirement: {req}
-Criteria:  Use correct punctuation. 
-Examples:  Unacceptable: The Navigation_Beacon shall provide Augmentation_Data having the characteristics defined in &lt;ICD xyz&gt; to each Maritime_User, engaged in Harbor_Harbor_Approach_Maneuvering (HHA) at an accuracy of less than 20 meters. [This is unacceptable because the incorrectly placed comma in this sentence confuses the meaning, leading the reader to believe that the accuracy is related to the maneuver rather than to the augmentation data.] Improved: The Navigation_Beacon shall provide Navigation_Data having the characteristics defined in &lt;ICD xyz&gt; to each Maritime_User engaged in Harbor_Harbor_Approach_Maneuvering (HHA), at an accuracy of less than 20 meters. [The positioning of the comma now makes it clear that the accuracy and availability relate to the data. Also note that, while performance measures are included, the appropriate conditions are not addressed. Further “Navigation_Beacon”, “Navigation_Data”, “Maritime_User”, and “Harbor_Harbor_Approach_Maneuvering (HHA)” must be defined in the glossary or data dictionary.] Guide to Writing Requirements 82 4</t>
+Criteria:
+ Express the propositional nature of a condition explicitly for a single action instead of giving lists of actions for a specific condition. 
+Examples:
+ Guide to Writing Requirements 98 Unacceptable: The Audit _Clerk shall be able to change the status of the action item when: - the Audit _Clerk originated the item; - the Audit _Clerk is the actionee; and - the Audit _Clerk is the reviewer. [This is unacceptable because it is not clear whether all the conditions must hold (a conjunction) or any one of them (a disjunction). Also, the requirement contains the phrase “be able to” which violates R11.] Better: If the requirement is interpreted as a disjunction: The Audit_System shall change the Action_Item status requested by the Audit_Clerk when one or more of the following conditions are true: - the Audit_Clerk originated the Action_Item; - the Audit_Clerk is the Actionee; or - the Audit_Clerk is the Reviewer. [Although the requirement is now improved, there is still the issue of verification. If the status does not change with one of the listed conditions, then the entire requirement fails verification, even if the other two conditions are met as specified.] Better: In this case, it would be best to state three distinct requirements as this makes each atomic and retains the same overall intent. From an allocation, traceability, and verifiability perspective this form is preferable. The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the Audit_Clerk originated the Action_Item. The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the Audit_Clerk is the Actionee. The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the Audit_Clerk is the Reviewer. Better if interpreted as a conjunction: The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the following conditions are true: - the Audit_Clerk originated the Action_Item AND - the Audit_Clerk is the Actionee AND - the Audit_Clerk is the Reviewer. [In this form, the three conditions are expressed as a logical condition such that all three must all be true for the logical condition to be true.] 4.8 Uniqueness 4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ Classify needs and requirements according to the aspects of the problem or system it addresses. 
+Examples:
+ Example classifications: Functional, Performance, Operational, Reliability, Availability, Maintainability, Safety, Security, Design and Construction Standards, Physical Characteristics. See the NRM for more guidance on organizing needs and requirements. See Also R41 – Related Requirements 4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ Express each need and requirement once and only once. 
+Examples:
+ Exact duplicates can be found by matching of text strings. The main problem is to identify similarities with different expressions, but which are equivalent. For example, the following statements are overlapping in that the first is a subset of the second: The &lt;SOI &gt; shall generate a report of financial transactions containing the information defined in &lt;some standard or contract deliverable listing&gt;. The &lt;SOI&gt; shall generate a financial report. 4.9 Abstraction 4</t>
   </si>
   <si>
     <t xml:space="preserve">Requirement: {req}
-Criteria:  Use a defined convention to express logical expressions such as “[X AND Y]”, “[X OR Y]”, [X XOR Y]”, “NOT [X OR Y]”. 
-Examples:  Unacceptable: The Engine_Management_System shall disengage the Speed_Control_Subsystem within &lt;TBD seconds&gt; when the Cruise_Control is engaged, and the Driver applies the Accelerator. [This is unacceptable because of the ambiguity of “and” could be confused with combining two separate thoughts. Instead use the form of a logical expression [X AND Y].] Improved: When [the Cruise_Control is Engaged] AND [the Accelerator is Applied], the Engine_Management_System shall Disengage the Speed_Control_Subsystem within &lt;TBD seconds&gt;. [“Engine_Management_System”, “Speed_Control_Subsystem”, “Disengage”, “Engaged”, “Accelerator”, “Applied”, and “Cruise_Control” must be defined in the glossary or data dictionary.] Guide to Writing Requirements 83 </t>
+Criteria:
+ Avoid stating implementation in a need statement or requirement statement unless there is rationale for constraining the design. 
+Examples:
+ General: For a medical diagnostic system • Stakeholders need statement: “The &lt;stakeholders&gt; need the &lt;diagnostic system&gt; to measure [something] with an accuracy as good as or better than similar devices in the market.” [This is an appropriate level of abstraction for a stakeholder need statement, clearly stating the expectation the stakeholders have concerning accuracy, however this would not be a good design input requirement.] • Requirement transformed from the stakeholder need statement: “The &lt;diagnostic system&gt; shall measure [something] with an accuracy of [xxx].” [The developers have explored various concepts for meeting the need for accuracy, have examined candidate technologies, have accessed their maturity (technology readiness level (TRL), and have decided that the value [xxx] is feasible with acceptable risk for this lifecycle stage. As stated, this is an appropriate level of detail for a design input requirement.] Note that when dealing with measures, both accuracy and precision must be addressed, either as separate requirements or including both in a measurement requirement defining characteristics of the measured parameter. These system-level design input accuracy and precision requirements are then allocated to the parts of the system architecture that have a role in meeting the overall system accuracy and precision requirements. For a medical diagnostic system this could include allocations to the hardware (instrument), assay (biological sample), and software. These allocations could then be further sub-allocated within the hardware, assay, and software lower-level entities. As long as the requirements are written on the accuracy and precision allocations and not how that accuracy or precision will be obtained by one of the architectural entities, the requirements are Design Input Requirements. As soon as specific hardware components are named (laser, LEDs emitting light at a specific wavelength, optical system components, specific magnifications, algorithms, formulations, etc.,) then the requirements are reflecting design outputs and need to be communicated within design output artifacts (specifications). Unacceptable: Traffic lights shall be used to control traffic at the intersection. [This is unacceptable because “Traffic lights” are a solution (design output). Why are traffic lights needed? This requirement is also written in passive voice - see R2] Improved: (several requirements): When a Pedestrian signals an intent to cross the street at the Intersection, the Traffic_Control_System shall provide [the Pedestrian a “Walk” signal AND provide the traffic a “Stop” signal]. The Traffic_Control_System shall limit the Wait_Time of Vehicles traversing the Intersection to less than Daylight_Wait_Time during Normal_Daytime traffic conditions. [Note that glossary definitions should be used for Traffic_Control_System, Daylight_Wait_Time_Value, Normal_Daytime, Vehicles, and Intersection.] Unacceptable: When a pedestrian signals his presence by pressing a button on the traffic-light pillar, the traffic light shall turn red for the traffic to stop. [This is unacceptable because this requirement contains solution-biased detail - design output. In addition, the requirement is unacceptable because it has additional information concerning Guide to Writing Requirements 102 the action traffic is to take and does not specify the duration of the red light. The use of a pronoun is also not recommended]. Improved: When the presence of a Pedestrian that needs to cross the street at the Intersection during Day_Light_Hours is detected, the Traffic_Control_System shall issue a Traffic_Stop_Signal for Average_Pedestrian_Crossing_Time. [This design input requirement allows freedom in determining the best solution (design output), which may be a means of automatic detection rather than button pushing along with the type and characteristics of the signal issued. Note that pedestrians may be in proximity of the intersection that do not wish to cross the street.] [An interesting consideration from a consistency or conflict perspective, what if the Average_Pedestrian_Crossing_Time” is greater than the “Daylight_Wait_Time_Value” defined for the traffic in the previous example. Each time is from a different entity perspective.] [Note that glossary definitions should be used for “Pedestrian”, “Traffic_Control_System”, “Traffic_Stop_Signal”, “Day_Light_Hours”, “Average_Pedestrian_Crossing_Time”, and “Intersection”.] </t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ Use “each” instead of “all”, “any”, or “both” when universal quantification is intended. 
+Examples:
+ Unacceptable: The Operation_Logger shall record any (or all) warning messages. [This is unacceptable because of the use of the word “any”, which is then made worse by the addition of “(or all)”.] Improved: The Operation_Logger shall record each Warning_Message. [Note that Warning_Message must be defined in the glossary so that it is clear that the SOI only will record each defined Warning Message. Also, any conditions or performance must also be included in the requirements statement for it to be complete.] Unacceptable: The Record_Subsystem shall display per &lt;Display Standard xyz&gt; the Names of both of the Line_Items. [This is unacceptable because of the use of the word “both”.] Improved: The Record_Subsystem shall display per &lt;Display Standard xyz&gt; the Name of each Line_Item. Improved: The Record_Subsystem shall display per &lt;Display Standard xyz&gt; each Line_Item_Name. 4.11 Tolerance 4</t>
   </si>
   <si>
     <t xml:space="preserve">Requirement: {req}
-Criteria:  Avoid the use of the word “not”. 
-Examples:  Unacceptable: The &lt;SOI&gt; shall not fail. [This is unacceptable because verification of the requirement would require infinite time. The requirement is also infeasible in that, as written, the implication is to never fail, under any conditions.] Improved: The &lt;SOI&gt; shall have an Availability of greater than or equal to 95%. or The &lt;SOI&gt; shall have a Mean Time Between Failures (MTBF) of xx operating hours. [For quality requirements, it would be more precise in the above were written as need statements. Then those transforming the quality need statements into requirement statements would define feasible concepts that would result in the needed quality attributes and derive well- formed requirements on the &lt;SOI&gt; that would result in those needs to be met.] Unacceptable: The &lt;SOI&gt; shall not contain mercury. [This is unacceptable because verification of the requirement would require the ability to measure the amount of mercury with infinite accuracy and precision. In addition, the real requirement may not be stated, for example, the real concern may be the use of toxic materials, not just mercury. If that is the case, it may be best to reference a standard from a governmental agency concerning allowable exposures to a list of common toxic materials.] Improved: The &lt;SOI&gt; shall limit metallic mercury exposure to those coming in contact with the &lt;SOI&gt; to less than or equal 0.025 mg/m3 over a period of 8 hours. </t>
+Criteria:
+ Define each quantity with a range of values appropriate to the entity to which the quantity applies and against which the entity will be verified or validated. Guide to Writing Requirements 104 
+Examples:
+ Unacceptable: The Pumping_Station shall maintain the flow of water at 100 liters per second for 30 minutes. [This is unacceptable because we do not know whether a solution that addresses more or less than the specified quantities is acceptable Also, it is not clear under what conditions this applies – when in operations, when powered on, when commanded?] Improved: When in operations, the Pumping_Station shall maintain Water_Flow at 100 ±10 liters for a minimum of 30 minutes. [Now the range of acceptable flow performance is clear and that the 30 minutes is a minimum acceptable performance. Given that the condition “when in operations”, this requirement applies whenever the Pumping_Station is active—no matter how long. Also, a question to be asked is what is the intent for how long—31 minutes satisfies the requirement, but what if the real intent is for however long the Pumping Station is in operations which could be hours or days – again depending on the operating conditions and need. What if there is not enough water at the inlet to the pumping station to establish the required flow rate?] Unacceptable: The Flight_Information_System shall display the current altitude to approximately 1 meter resolution. [This is unacceptable because it is imprecise. What is “approximately” in the context of a distance of 1 meter? Who has the option of deciding what is “approximately”? How will “approximately” be verified? What is the acceptable tolerance?] [Note that care must be taken to confirm that the units are appropriate in the context of the organizational and project templates. See also R6.] Improved: The Flight_Information_System shall display Current_Altitude with an accuracy of ±1 meter. [Note that “Current_Altitude” must be defined in the glossary since there are a number of possible interpretations of the term.] Unacceptable: The &lt;SOI&gt; shall limit arsenic contamination in the drinking water to allowable levels. Rationale: Arsenic contamination in drinking water can cause health problems. [While “allowable” is acceptable in a need statement, it is unacceptable in a requirement statement because allowable is ambiguous - allowable by whom? What specific concentration is allowable? In what market?] Unacceptable: The &lt;SOI&gt; shall limit arsenic contamination in the drinking water to 1 part per trillion. Rationale Attribute (A1): Arsenic contamination in drinking water can cause health problems. [This is unacceptable because the EPA contamination limit in drinking water is 10 parts per billion. Requiring a tighter limit may be beyond the ability of current technology to measure or if measuring concentrations of 1 part per trillion are possible, the cost to do so may be unacceptably high. Also, no range is specified. Using ‘less than’ is probably the real intent.] Improved: The &lt;SOI&gt; shall limit arsenic contamination in the drinking water to less than10 parts per billion. Rationale Attribute (A1): EPA set the arsenic standard for drinking water at 10 ppb (or 0.010 parts per million). The EPA has determined that concentrations of this level or less will protect consumers from the effects of long-term, chronic exposure to arsenic. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement: {req}
+Criteria:
+ Provide specific measurable performance targets appropriate to the entity to which the need or requirement is stated and against which the entity will be verified to meet. 
+Examples:
+ Unacceptable: The &lt;SOI&gt; shall use minimum power. [This is unacceptable because both words “use” and “minimum” are ambiguous and unverifiable.] Improved: The &lt;SOI&gt; shall consume less than or equal to 50W of mains power. [This both considers the underlying goal—to minimize power consumption—and provides a measurable target.] Unacceptable: The engine shall achieve an emissions level that is at least 5% less than the competition’s emission levels 2 years from now. [This is an actual requirement from marketing to an engineering department. The statement sets a completely unmeasurable end state.] Improved: The Engine shall achieve an emissions level that is less than or equal to xxx. [where xxx represents the required threshold value, including the appropriate units.] Unacceptable: The &lt;SOI&gt; shall conform to best practices for spurious emissions. [This statement is vague and unverifiable from number of specifics] Improved: The &lt;SOI&gt; shall limit Spurious_Emissions in accordance with &lt;Clause xab of Standard XYZ&gt;. </t>
   </si>
   <si>
     <t>Requirement: {req}
-Criteria:  Avoid the use of the oblique (“/”) symbol. 
-Examples:  Unacceptable: The User_Management_System shall Open/Close the User_Account in less than 1 second. [This is unacceptable because it is unclear as to what is meant by open/close: open, close, or both?] Improved: (Split into two requirements with an appropriate condition) When &lt;condition&gt;, the User_Management_System shall Open the User_Account in less than 1 second. When &lt;condition&gt;, the User_Management_System shall Close the User_Account in less than 1 second. Unacceptable: When the Clutch is Disengaged and/or the Brake is Applied, the Engine_Management_System shall disengage the Speed_Control_Subsystem within &lt;XYZ ms&gt;. [This is unacceptable because of the use of “and/or.” If simultaneity is intended—that is the dual conditions must be met at the same time—write the requirements as a logical AND. If “and” is meant in the sense that the action is to be completed under each of the conditions, split the two thoughts into separate requirements, one for each condition. If “or” is meant, write the requirement as a logical OR.] Improved: (As one requirement if simultaneity is intended): When [the Clutch is Disengaged] AND [the Brake is Applied], the Engine_Management_System shall disengage the Speed_Control_Subsystem within &lt;XYZ ms&gt;. Guide to Writing Requirements 85 Improved: (As two requirements if two separate conditions are intended): When the Clutch is Disengaged, the Engine_Management_System shall disengage the Speed_Control_Subsystem within &lt;XYZ ms&gt;. When the Brake is Applied, the Engine_Management_System shall disengage the Speed_Control_Subsystem within &lt;XYZ ms&gt;. Improved: (As one requirement if inclusive OR is intended) When EITHER [the Clutch is Disengaged] OR [the Brake is Applied], the Engine_Management_System shall disengage the Speed_Control_Subsystem. 4.4 Singularity 4</t>
+Criteria:
+ Define temporal dependencies explicitly instead of using indefinite temporal keywords such as “eventually”, “until”, “before”, “after”, “as”, “once”, “earliest”, “latest”, “instantaneous”, “simultaneous”, and “at last”. 
+Examples:
+ Unacceptable: Continual operation of the pump shall eventually result in the tank being empty. [This is unacceptable because “eventually” is ambiguous. Also, this statement is not written in the proper form. It is written on “operation” rather than on a requirement on the pump which violates R3.] Improved: The Pump shall remove greater than 99% of the Fluid from the Tank in less than 3 days of continuous operation. 4.13 Uniformity of Language 4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ Use each term and unit of measure consistently throughout need and requirement sets as well as associated models and other SE artefacts developed across the lifecycle. 
+Examples:
+ Unacceptable: It would not be acceptable for one requirement to refer to an entity using one term and another to refer to the same entity using another term. For example, a subsystem set of Design Input Requirements contains the following three requirement statements: The Radio shall .... The Receiver shall .... The Terminal shall .... Or: The Bleed_Valve shall .... The High-Pressure_Bleed_Valve shall .... The HPBV shall .... If each term refers to the same subject, the statements need to be modified to use the same word (or, if they are meant to be different, the words must be defined to be so). Improved: Settle on only one term, define it in the glossary or data dictionary, and then use it consistently in each need, requirement, and design output artifact. Unacceptable: When the Input_Valve is connected to the Water_Source, the Control_Subsystem shall open the Inlet_Valve. [Two terms are used for the same thing “Input_Valve” and “Inlet_Valve”.] Improved: When the Inlet_Valve is connected to the Water_Source, the Control_Subsystem shall open the Inlet_Valve. Unacceptable: It would not be acceptable for one requirement to use one unit of measure (for example, US - feet) and another requirement to use another unit of measure (for example, Metric - meter). Guide to Writing Requirements 109 Improved: Settle on which units of measure will be used and use that unit of measure consistency across all SE artifacts including needs, Design Input Requirements and design output specifications. Also, see R40 for guidance regarding the conversion from one measurement system to another and the use of significant digits. 4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ If acronyms are used, they must be consistent throughout need and requirement sets as well as associated models and other SE artefacts developed across the lifecycle. 
+Examples:
+ Unacceptable: It would not be acceptable for one requirement to use the acronym “CP” for command post and another acronym “CMDP” to also refer to the “command post.” The use of two different acronyms implies that the two system elements being referred to are different. Improved: Settle on only one acronym, define it in the list of acronyms, and then use it consistently throughout the requirement set. Unacceptable: It would not be acceptable for one requirement to refer to the “Global Positioning System” and the remaining requirements refer just to “GPS.” Improved: Use the full term every time or, perhaps more usefully, define the acronym in the project acronym list or glossary and use it every time. 4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ Avoid the use of abbreviations in needs and requirement statements as well as associated models and other SE lifecycle artefacts. Guide to Writing Requirements 110 
+Examples:
+ Unacceptable: It would not be acceptable for one requirement to refer to the abbreviation “op” meaning operation and another to refer to the “op” meaning the operator. Improved: Avoid the abbreviation and use the full term every time. 4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ Use a project-wide style guide for individual need statements and requirement statements. 
+Examples:
+ For example, each organization should have a style guide or schema to address such issues as the selection and definition of what need patterns and requirement patterns should be used for writing need statements and requirement statements of a particular type, the selection and use of attributes, standard abbreviations and acronyms, layout and use of figures and tables, layout of documents or databases and, statement numbering. Guide to Writing Requirements 111 Terms used throughout the sets of needs and sets of requirements are defined in an ontology or at least a project glossary. 4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ Use a consistent format and number of signification digits for the specification of decimal numbers. 
+Examples:
+ Unacceptable: The &lt;SOI&gt; shall have an MTBF of less than or equal to 9.499,99 h. &amp; The &lt;SOI&gt; shall consume less than or equal to 0.99 W. [These two statements are unacceptable when included in the same set because a different format is used in the two statements.] Improved: The &lt;SOI&gt; shall have an MTBF of less than or equal to 9,499.99 h. &amp; The &lt;SOI&gt; shall consume less than or equal to 0.99 W. OR The &lt;SOI&gt; shall have an MTBF of less than or equal to 9.499,99 h. &amp; The &lt;SOI&gt; shall consume less than or equal to 0,99 W. Unacceptable: The &lt;SOI&gt; shall have an MTBF of less than or equal to 0.99 h. &amp; The &lt;SOI&gt; shall consume less than or equal to .99 W. [These two statements are unacceptable when included in the same set because a different format is used in the two statements.] Improved: The &lt;SOI&gt; shall have an MTBF of less than or equal to 9,499.99 h. &amp; The &lt;SOI&gt; shall consume less than or equal to 0.99 W. 4.14 Modularity 4</t>
+  </si>
+  <si>
+    <t>Requirement: {req}
+Criteria:
+ Group related needs and requirements together. 
+Examples:
+ Requirements may be related by: - type (for example, critical functions, enabling functions, safety, or security requirements); - scenario (for example, requirements arising from a single scenario). - interactions with other systems (for example interface requirements). - function (for example, multiple requirements defined for a function, each addressing a different performance characteristics, mode, state, condition, or trigger.) - capability (for example a needed capability may be released by a set of requirements that together result in the needed capability to be provided. -compliance (for example requirements whose purpose it is to implement a requirement in a standard or regulation. See R29 and the NRM for more guidance on organizing needs and requirements. 4</t>
   </si>
   <si>
     <t xml:space="preserve">Requirement: {req}
-Criteria:  Write a single sentence that contains a single thought conditioned and qualified by relevant sub- clauses. 
-Examples:  Unacceptable: When in the Active_State, the Record_Subsystem shall display the Name of each Line_Item and shall record the Location of each Line_Item, without obscuring the User_ID. [This is unacceptable because the sentence contains two requirements and the qualification only applies to the first requirement, not the second.] Improved: (Split into two separate requirements) When in the Active_State, the Record_Subsystem shall display per &lt;Display Standard XYZ&gt; the Name of each Line_Item, without obscuring the User_ID. When in the Active_ State, the Record_Subsystem shall record the Location of each Line_Item. [Note use of the glossary or data dictionary to define terms. Any applicable performance measures must be addressed for the requirement to be complete.] Unacceptable: The Control_Subsystem will close the Inlet_Valve until the temperature has reduced to 85 °C, when it will then reopen it in less than 1 second. [This is unacceptable because the sentence contains two event driven requirements. Additionally, the sentence contains two occurrences of the pronoun “it” ambiguously referring to different things (see R26), the term “has reduced” is ambiguous, and the action verb must be ”shall”, not “will”. Also, a time constraint is included but it is not clear whether it applies to both actions or only the second action.] Improved: (Split into two requirements each with its own time constraint): If the Water_Temperature in the Boiler increases to greater than 85 °C, the Control_Subsystem shall close the Inlet_Valve in less than 1 second. When the Water_Temperature in the Boiler reduces to less than or equal to 85 °C, the Control_Subsystem shall open the Inlet_Valve in less than 1 second. [Note use of the glossary or data dictionary to define terms.] Unacceptable: In the event of a fire detection, within &lt;xxx ms&gt;: • Security entrances shall be set to Free_Access_Mode. • Fire escape doors shall be unlocked. [This is unacceptable because the condition “in the event of a fire detection” is stated following a list of actions to be taken; each of which the system must be verified against. Also, note the actions are written in passive voice which violates R2. Each action needs to be communicated in a separate active voice requirement statement. For multiple conditions for a single action see R28.] Improved: (Split into two requirements) In the event of Fire_Detection, the Fire_Control_Subsystem shall set the Free_Access_Mode to ON within &lt;xxx ms&gt;. In the event of Fire_Detection, the Fire_Control_Subsystem shall send the Fire_Door_Unlock unlock command having the characteristics defined in &lt;ICD xyz&gt; to each Fire_Door within &lt;xxx ms&gt;. [There is a Fire Detection subsystem responsible for detecting fires and setting the Fire_Detection parameter to “TRUE” which triggers the two actions. All other subsystems that Guide to Writing Requirements 87 are monitoring when the Fire_Control_Subsystem has set the Free_Access_Mode to “TRUE” will take the required action as stated in their set of requirements. All Fire Doors will be monitoring for the Fire_Door_Unlock command and will unlock when the command is received.] Unacceptable: The &lt;corporate website&gt; shall use only approved fonts. The approved fonts are: &lt;Font1&gt;, &lt;Font2&gt; and &lt;Font3&gt;. [This is unacceptable because it is non-singular. Rather than splitting into three requirements (which is quite difficult to so whilst conforming to the “only” constraint, the term “Approved_Fonts” can be included in the Glossary, which then states: “Approved_Fonts: &lt;Font1&gt;, &lt;Font2&gt; and &lt;Font3&gt;.”] Improved: (using the glossary term “Approved_Fonts”) The &lt;corporate website&gt; shall use only Approved_Fonts. [Alternately, the organization can define a display standard which includes a definition of approved fonts, and the requirement could reference that standard.] Improved: (referring to a standard.) The &lt;corporate website&gt; shall display information in accordance with &lt;Display Standard xyz&gt;. [Note that this also allows better configuration management of the requirements database, particularly if the approved fonts are referred to in a number of requirements—that is, should the approved fonts change or characteristics of the fonts change, the list of approved fonts and characteristics only needs to be updated in the Glossary, rather than in multiple requirements (in which case there is a risk that one or more of the requirements is missed).] [In reality, requirements involving the actions such as “display” are interface requirements given that the information will be provided by something to some display device for display.] [Having the information in the display standard then can be referred to in the set of requirements for that display device. Note that referring to a standard also allows for later specialization, for example different parts of the standard may apply to different display devices.] </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requirement: {req}
-Criteria:  Avoid words that join or combine clauses, such as “and”, “or”, “then”, “unless”, “but”, “as well as” “but also”, “however”, “whether”, “meanwhile”, “whereas”, “on the other hand”, or “otherwise”. 
-Examples:  Unacceptable: The user shall either be trusted or not trusted. [This is unacceptable for several reasons. The intention is that a user should be classified in one of two ways, but it is also a passive requirement written on the user rather than on the system (R2) and it is ambiguous: the requirement would still be met if the system took the option of treating all users as trusted.] Improved: The Security_System shall categorize each User as EITHER Trusted OR Not_Trusted. Unacceptable: The &lt;SOI&gt; shall display the Location and Identity of the Lead_Vehicle. [This is unacceptable because is in fact stating two requirements which may well need to be verified by different verification actions. In addition, the format of the displayed information is not referenced.] Improved: (Express as two requirements) The &lt;SOI&gt; shall display the Location of the Lead_Vehicle per &lt;Display Standard xyx&gt;. The &lt;SOI&gt; shall display the Identity of the Lead_Vehicle per &lt;Display Standard xyx&gt;. Unacceptable: The &lt;SOI&gt; shall provide an audible or visual alarm having the characteristics defined in &lt;alarm standard xyz&gt;. [This is unacceptable because it is a moot point as to whether the designer can choose which alarm to implement, or (which is probably the intent of the writer) whether both alarms are required, and the operator is alerted by at least one.] Improved: (if the choice is available to the designer) The &lt;SOI&gt; shall provide EITHER an Audible_Alarm OR Visual_Alarm having the characteristics defined in &lt;Alarm Standard xyz&gt;. Improved: (if both alarms are required) Guide to Writing Requirements 89 The &lt;SOI&gt; shall provide an Audible_Alarm having the characteristics defined in &lt;Alarm Standard xyz&gt;. The &lt;SOI&gt; shall provide a Visual_Alarm having the characteristics defined in &lt;Alarm Standard xyz&gt;. [As separate requirements, each can be allocated differently, and the SOI will be verified to meet each. </t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  Avoid phrases that indicate the “purpose of “, “intent of”, or “reason for” the need statement or requirement statement. 
-Examples:  Unacceptable: The Record_Subsystem shall display the Name of each Line_Item so that the Operator can confirm that it is the correct Item. [This is unacceptable because the text “so that the Operator can confirm that it is the correct Item” is rationale.] Improved: The Record_Subsystem shall display the Name of each Line_Item per &lt;Display Standard XYZ&gt;. [The text “so that the Operator can confirm that it is the correct Item” should be included in the rationale attribute.] Guide to Writing Requirements 90 Unacceptable: The Operation_Logger shall record each Warning_Message produced by the system. [This is unacceptable because of the superfluous words “produced by the system”.] Improved: The Operation_Logger shall record each Warning_Message within &lt;performance measure&gt;. 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requirement: {req}
-Criteria:  Avoid parentheses and brackets containing subordinate text. 
-Examples:  Unacceptable: When the Water_Temperature exceeds 85 °C (usually towards the end of the boiling cycle), the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt; [This is unacceptable because of the parenthetical phrase as well as the ambiguous word “usually”. Note that the parameter Water_Temperature needs to be defined in the glossary in order to be specific] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt;. [Note: for the above example, if this behavior is the result of a design decision, then the requirement needs to be communicated as a design output. The design input requirement should focus on why this behavior is needed - for example, prevent the boiler from over pressurizing and exploding. This is a good example of the benefit of asking “Why” for requirements of this type. The answer is the real design input requirement. If included in the set of Design Input Requirements, then the “why” should be included in the rationale.] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall prevent the Boiler from over pressurization. [How this is done is a design decision.} </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requirement: {req}
-Criteria:  Enumerate sets explicitly instead of using a group noun to name the set. 
-Examples:  Unacceptable: The thermal control system shall manage temperature-related functions. [This is unacceptable because there is ambiguity regarding which functions are to be managed as well as what is meant by “managed”. The specific functions should be enumerated explicitly in separate requirement statements along with performance expectations and any applicable conditions, triggers, or constraints.] Unacceptable: The thermal control system shall monitor system temperature. This is unacceptable because there is ambiguity regarding the function “monitor”. Similar to “managed” What are the expectations of the stakeholders – update the display of the system temperature, maintain the temperature within some range, or store the history of the system temperature? The specific subfunctions should be enumerated explicitly in separate requirement statements along with performance expectations and any applicable conditions, triggers, or constraints.] Improved: (three separate requirements): The Thermal_Control_System shall update the display of System_Temperature every 10 +/- 1 seconds. The Thermal_Control_System shall maintain the System_Temperature between 95°C and 98°C. The Thermal_Control_System shall store the history of System_Temperature. [Note use of the glossary to define terms.] </t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  When a need or requirement is related to complex behavior, refer to a supporting diagram, model, or ICD. 
-Examples:  Unacceptable: The Control_System shall close Valves A AND B within 5 seconds of the temperature exceeding 95 °C AND within 2 seconds of each other. [This is unacceptable because of the confusing set of conditions. In this case what is meant will be clear if the requirement referred to a diagram for context.] Improved: [Within 5 seconds of the temperature exceeding 95 °C] AND [within 2 seconds of each other as shown in Timing_Diagram_6], the Control_System shall close [Valve A AND Valve B]. [Note that this assumes, of course, that the timing diagram itself is not ambiguous. If it is not possible to remove the ambiguity by using a diagram, it may be better to split the requirement into two.] [Note: for the above example, if this complex behavior is the result of a design decision, then the requirement needs to be communicated as a design output. The design input requirement should focus on why this behavior is needed.] Interface Example: An interface requirement may refer to the characteristics of the electrical power (current/voltage) being supplied by a system. There can be multiple characteristics that need to be defined such that the systems receiving the power have a clear understanding of the characteristics of the power they are receiving. In this case it is common for the characteristics to be defined in an ICD which both the provider and receiver of the power can refer to in their Design Input Requirements. From the provider perspective the provider system will have to be verified that the power provided has all of these characteristics and the receiver will have to verify it can receive and operate on power having these same characteristics. &lt;System 1&gt; shall provide power to &lt;System 2&gt; having the characteristics defined in &lt;ICD xyz&gt;. Table 123&gt;. &lt;System 2&gt; shall receive power from &lt;System 1&gt; having the characteristics defined in &lt;ICD xyz&gt;. Table 123&gt;. &lt;System 2&gt; shall operate on power having the characteristics defined in &lt;ICD xyz&gt;. Table 123&gt;. 4.5 Completeness 4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  Avoid the use of personal and indefinite pronouns. 
-Examples:  Unacceptable: The controller shall send the driver his itinerary for the day. It shall be delivered at least 8 hours prior to his Shift. [This is unacceptable because the requirement is expressed as two sentences and the second sentence uses the pronouns “it” and “his.”] Improved: At least 8 hours prior to the Driver_Shift, the Controller shall send the Driver_Itinerary for the day to the Driver. [Note use of the glossary to define terms and to be explicit about the relationship between the driver, shift, and the itinerary for that particular driver.] 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requirement: {req}
-Criteria:  Avoid relying on headings to support explanation or understanding of the need or requirement. 
-Examples:  Example heading: “4.0 Alert Buzzer Requirements.” Unacceptable: 4.1 The &lt;SOI&gt; shall sound it for greater than 20 minutes. [This is unacceptable because the requirement uses the pronoun “it” (R24), which requires the heading to understand what “it” means. In addition, the word “sound” could be ambiguous as it can be a noun, a verb, adverb, or adjective. We do not know whether Alert_Buzzer is a subsystem that controls the noise or the thing that makes the noise.] Improved: When &lt;triggering event&gt;, the &lt;SOI&gt; shall sound an alert having the characteristics defined in &lt;Alert Standard xyz&gt; for greater than 20 minutes. [In this improved rewrite, the existence of the header is not needed to interpret the requirement. Even though the above heading referenced an “Alert Buzzer”—an implementation, the improved requirement avoids implementation to a specific device, and rather indicates that when the triggering event happens, an alert is required to be sounded having the characteristics defined in the alert standard. </t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  Avoid using unachievable absolutes. 
-Examples:  Unacceptable: The &lt;SOI&gt; shall have 100% availability. [This is unacceptable because 100% is an absolute that is impossible to achieve and verify. Also, available over what time period?] Improved: The &lt;SOI&gt; shall have an Availability of greater than or equal to 98% during Operating_Hours. [Note use of the glossary to define Operating_Hours. Alternatively, this requirement could be stated as a need. Then those transforming the need into requirements would develop a Guide to Writing Requirements 96 feasible concept for doing so and then derive specific Design Input Requirements that would result in the need being met.] Unacceptable: The Pumping_Station shall maintain the flow of water at 100 liters per second for 30 minutes. [This is unacceptable because the requirement is impossibly precise to maintain in terms of the flow rate (and impossibly precise to measure in verification) as well as being impossibly precise to deliver for 30 minutes exactly. Also, it is not clear under what conditions this applies—when in operations, when powered on, when commanded?] Improved: When in operations, the Pumping_Station shall maintain Water_Flow at 100 ±10 liters per second for greater than 30 minutes. [Now the range of acceptable flow performance and time frame is clear and feasible. Given that the condition “when in operations” this requirement applies whenever the Pumping_Station is active—no matter how long. Also, what is the intent for how long—31 minutes satisfies the requirement, but what if the real intent is for however long the Pumping Station is in operations which could be hours or days—again depending on the operating conditions and need. Further, is the 30 minutes of continuous flow or a total of 30 minutes within a set time period?] 4.7 Conditions 4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  State conditions’ applicability explicitly instead of leaving applicability to be inferred from the context. 
-Examples:  Unacceptable: The Free_Access_Mode shall be set to ON within &lt;xxx ms&gt;. The Fire_Door_Unlock command having the characteristics defined in &lt;ICD xyz&gt; shall be sent to each Fire_Door within &lt;xxx ms&gt;. [This is unacceptable because the condition or trigger for these actions is not stated. Also, note the actions are written in passive voice which violates R2. Each action needs to be communicated in a separate active voice requirement statement with the condition or trigger for which the action is to be initiated. For multiple conditions for a single action see R28.] Improved: (Split into two requirements) In the event of Fire_Detection, the Fire_Control_Subsystem shall set the Free_Access_Mode to ON within &lt;xxx ms&gt;. In the event of Fire_Detection, the Fire_Control_Subsystem shall send the Fire_Door_Unlock unlock command having the characteristics defined in &lt;ICD xyz&gt; to each Fire_Door within &lt;xxx ms&gt;. [Note that there is a Fire Detection subsystem responsible for detecting fires and setting the Fire_Detection parameter to “TRUE” which triggers the two actions. All other subsystems that are monitoring when the Fire_Control_Subsystem has set the Free_Access_Mode to “TRUE” will have their own requirements to monitor this parameter and take the required action(s) as stated in their set of requirements. All Fire Doors will have their own requirements to monitor for the Fire_Door_Unlock command and to unlock when the command is received.] 4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  Express the propositional nature of a condition explicitly for a single action instead of giving lists of actions for a specific condition. 
-Examples:  Guide to Writing Requirements 98 Unacceptable: The Audit _Clerk shall be able to change the status of the action item when: - the Audit _Clerk originated the item; - the Audit _Clerk is the actionee; and - the Audit _Clerk is the reviewer. [This is unacceptable because it is not clear whether all the conditions must hold (a conjunction) or any one of them (a disjunction). Also, the requirement contains the phrase “be able to” which violates R11.] Better: If the requirement is interpreted as a disjunction: The Audit_System shall change the Action_Item status requested by the Audit_Clerk when one or more of the following conditions are true: - the Audit_Clerk originated the Action_Item; - the Audit_Clerk is the Actionee; or - the Audit_Clerk is the Reviewer. [Although the requirement is now improved, there is still the issue of verification. If the status does not change with one of the listed conditions, then the entire requirement fails verification, even if the other two conditions are met as specified.] Better: In this case, it would be best to state three distinct requirements as this makes each atomic and retains the same overall intent. From an allocation, traceability, and verifiability perspective this form is preferable. The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the Audit_Clerk originated the Action_Item. The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the Audit_Clerk is the Actionee. The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the Audit_Clerk is the Reviewer. Better if interpreted as a conjunction: The Audit_System shall change the Action_Item status requested by the Audit_Clerk when the following conditions are true: - the Audit_Clerk originated the Action_Item AND - the Audit_Clerk is the Actionee AND - the Audit_Clerk is the Reviewer. [In this form, the three conditions are expressed as a logical condition such that all three must all be true for the logical condition to be true.] 4.8 Uniqueness 4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  Classify needs and requirements according to the aspects of the problem or system it addresses. 
-Examples:  Example classifications: Functional, Performance, Operational, Reliability, Availability, Maintainability, Safety, Security, Design and Construction Standards, Physical Characteristics. See the NRM for more guidance on organizing needs and requirements. See Also R41 – Related Requirements 4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  Express each need and requirement once and only once. 
-Examples:  Exact duplicates can be found by matching of text strings. The main problem is to identify similarities with different expressions, but which are equivalent. For example, the following statements are overlapping in that the first is a subset of the second: The &lt;SOI &gt; shall generate a report of financial transactions containing the information defined in &lt;some standard or contract deliverable listing&gt;. The &lt;SOI&gt; shall generate a financial report. 4.9 Abstraction 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requirement: {req}
-Criteria:  Avoid stating implementation in a need statement or requirement statement unless there is rationale for constraining the design. 
-Examples:  General: For a medical diagnostic system • Stakeholders need statement: “The &lt;stakeholders&gt; need the &lt;diagnostic system&gt; to measure [something] with an accuracy as good as or better than similar devices in the market.” [This is an appropriate level of abstraction for a stakeholder need statement, clearly stating the expectation the stakeholders have concerning accuracy, however this would not be a good design input requirement.] • Requirement transformed from the stakeholder need statement: “The &lt;diagnostic system&gt; shall measure [something] with an accuracy of [xxx].” [The developers have explored various concepts for meeting the need for accuracy, have examined candidate technologies, have accessed their maturity (technology readiness level (TRL), and have decided that the value [xxx] is feasible with acceptable risk for this lifecycle stage. As stated, this is an appropriate level of detail for a design input requirement.] Note that when dealing with measures, both accuracy and precision must be addressed, either as separate requirements or including both in a measurement requirement defining characteristics of the measured parameter. These system-level design input accuracy and precision requirements are then allocated to the parts of the system architecture that have a role in meeting the overall system accuracy and precision requirements. For a medical diagnostic system this could include allocations to the hardware (instrument), assay (biological sample), and software. These allocations could then be further sub-allocated within the hardware, assay, and software lower-level entities. As long as the requirements are written on the accuracy and precision allocations and not how that accuracy or precision will be obtained by one of the architectural entities, the requirements are Design Input Requirements. As soon as specific hardware components are named (laser, LEDs emitting light at a specific wavelength, optical system components, specific magnifications, algorithms, formulations, etc.,) then the requirements are reflecting design outputs and need to be communicated within design output artifacts (specifications). Unacceptable: Traffic lights shall be used to control traffic at the intersection. [This is unacceptable because “Traffic lights” are a solution (design output). Why are traffic lights needed? This requirement is also written in passive voice - see R2] Improved: (several requirements): When a Pedestrian signals an intent to cross the street at the Intersection, the Traffic_Control_System shall provide [the Pedestrian a “Walk” signal AND provide the traffic a “Stop” signal]. The Traffic_Control_System shall limit the Wait_Time of Vehicles traversing the Intersection to less than Daylight_Wait_Time during Normal_Daytime traffic conditions. [Note that glossary definitions should be used for Traffic_Control_System, Daylight_Wait_Time_Value, Normal_Daytime, Vehicles, and Intersection.] Unacceptable: When a pedestrian signals his presence by pressing a button on the traffic-light pillar, the traffic light shall turn red for the traffic to stop. [This is unacceptable because this requirement contains solution-biased detail - design output. In addition, the requirement is unacceptable because it has additional information concerning Guide to Writing Requirements 102 the action traffic is to take and does not specify the duration of the red light. The use of a pronoun is also not recommended]. Improved: When the presence of a Pedestrian that needs to cross the street at the Intersection during Day_Light_Hours is detected, the Traffic_Control_System shall issue a Traffic_Stop_Signal for Average_Pedestrian_Crossing_Time. [This design input requirement allows freedom in determining the best solution (design output), which may be a means of automatic detection rather than button pushing along with the type and characteristics of the signal issued. Note that pedestrians may be in proximity of the intersection that do not wish to cross the street.] [An interesting consideration from a consistency or conflict perspective, what if the Average_Pedestrian_Crossing_Time” is greater than the “Daylight_Wait_Time_Value” defined for the traffic in the previous example. Each time is from a different entity perspective.] [Note that glossary definitions should be used for “Pedestrian”, “Traffic_Control_System”, “Traffic_Stop_Signal”, “Day_Light_Hours”, “Average_Pedestrian_Crossing_Time”, and “Intersection”.] </t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  Use “each” instead of “all”, “any”, or “both” when universal quantification is intended. 
-Examples:  Unacceptable: The Operation_Logger shall record any (or all) warning messages. [This is unacceptable because of the use of the word “any”, which is then made worse by the addition of “(or all)”.] Improved: The Operation_Logger shall record each Warning_Message. [Note that Warning_Message must be defined in the glossary so that it is clear that the SOI only will record each defined Warning Message. Also, any conditions or performance must also be included in the requirements statement for it to be complete.] Unacceptable: The Record_Subsystem shall display per &lt;Display Standard xyz&gt; the Names of both of the Line_Items. [This is unacceptable because of the use of the word “both”.] Improved: The Record_Subsystem shall display per &lt;Display Standard xyz&gt; the Name of each Line_Item. Improved: The Record_Subsystem shall display per &lt;Display Standard xyz&gt; each Line_Item_Name. 4.11 Tolerance 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requirement: {req}
-Criteria:  Define each quantity with a range of values appropriate to the entity to which the quantity applies and against which the entity will be verified or validated. Guide to Writing Requirements 104 
-Examples:  Unacceptable: The Pumping_Station shall maintain the flow of water at 100 liters per second for 30 minutes. [This is unacceptable because we do not know whether a solution that addresses more or less than the specified quantities is acceptable Also, it is not clear under what conditions this applies – when in operations, when powered on, when commanded?] Improved: When in operations, the Pumping_Station shall maintain Water_Flow at 100 ±10 liters for a minimum of 30 minutes. [Now the range of acceptable flow performance is clear and that the 30 minutes is a minimum acceptable performance. Given that the condition “when in operations”, this requirement applies whenever the Pumping_Station is active—no matter how long. Also, a question to be asked is what is the intent for how long—31 minutes satisfies the requirement, but what if the real intent is for however long the Pumping Station is in operations which could be hours or days – again depending on the operating conditions and need. What if there is not enough water at the inlet to the pumping station to establish the required flow rate?] Unacceptable: The Flight_Information_System shall display the current altitude to approximately 1 meter resolution. [This is unacceptable because it is imprecise. What is “approximately” in the context of a distance of 1 meter? Who has the option of deciding what is “approximately”? How will “approximately” be verified? What is the acceptable tolerance?] [Note that care must be taken to confirm that the units are appropriate in the context of the organizational and project templates. See also R6.] Improved: The Flight_Information_System shall display Current_Altitude with an accuracy of ±1 meter. [Note that “Current_Altitude” must be defined in the glossary since there are a number of possible interpretations of the term.] Unacceptable: The &lt;SOI&gt; shall limit arsenic contamination in the drinking water to allowable levels. Rationale: Arsenic contamination in drinking water can cause health problems. [While “allowable” is acceptable in a need statement, it is unacceptable in a requirement statement because allowable is ambiguous - allowable by whom? What specific concentration is allowable? In what market?] Unacceptable: The &lt;SOI&gt; shall limit arsenic contamination in the drinking water to 1 part per trillion. Rationale Attribute (A1): Arsenic contamination in drinking water can cause health problems. [This is unacceptable because the EPA contamination limit in drinking water is 10 parts per billion. Requiring a tighter limit may be beyond the ability of current technology to measure or if measuring concentrations of 1 part per trillion are possible, the cost to do so may be unacceptably high. Also, no range is specified. Using ‘less than’ is probably the real intent.] Improved: The &lt;SOI&gt; shall limit arsenic contamination in the drinking water to less than10 parts per billion. Rationale Attribute (A1): EPA set the arsenic standard for drinking water at 10 ppb (or 0.010 parts per million). The EPA has determined that concentrations of this level or less will protect consumers from the effects of long-term, chronic exposure to arsenic. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requirement: {req}
-Criteria:  Provide specific measurable performance targets appropriate to the entity to which the need or requirement is stated and against which the entity will be verified to meet. 
-Examples:  Unacceptable: The &lt;SOI&gt; shall use minimum power. [This is unacceptable because both words “use” and “minimum” are ambiguous and unverifiable.] Improved: The &lt;SOI&gt; shall consume less than or equal to 50W of mains power. [This both considers the underlying goal—to minimize power consumption—and provides a measurable target.] Unacceptable: The engine shall achieve an emissions level that is at least 5% less than the competition’s emission levels 2 years from now. [This is an actual requirement from marketing to an engineering department. The statement sets a completely unmeasurable end state.] Improved: The Engine shall achieve an emissions level that is less than or equal to xxx. [where xxx represents the required threshold value, including the appropriate units.] Unacceptable: The &lt;SOI&gt; shall conform to best practices for spurious emissions. [This statement is vague and unverifiable from number of specifics] Improved: The &lt;SOI&gt; shall limit Spurious_Emissions in accordance with &lt;Clause xab of Standard XYZ&gt;. </t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  Define temporal dependencies explicitly instead of using indefinite temporal keywords such as “eventually”, “until”, “before”, “after”, “as”, “once”, “earliest”, “latest”, “instantaneous”, “simultaneous”, and “at last”. 
-Examples:  Unacceptable: Continual operation of the pump shall eventually result in the tank being empty. [This is unacceptable because “eventually” is ambiguous. Also, this statement is not written in the proper form. It is written on “operation” rather than on a requirement on the pump which violates R3.] Improved: The Pump shall remove greater than 99% of the Fluid from the Tank in less than 3 days of continuous operation. 4.13 Uniformity of Language 4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  Use each term and unit of measure consistently throughout need and requirement sets as well as associated models and other SE artefacts developed across the lifecycle. 
-Examples:  Unacceptable: It would not be acceptable for one requirement to refer to an entity using one term and another to refer to the same entity using another term. For example, a subsystem set of Design Input Requirements contains the following three requirement statements: The Radio shall .... The Receiver shall .... The Terminal shall .... Or: The Bleed_Valve shall .... The High-Pressure_Bleed_Valve shall .... The HPBV shall .... If each term refers to the same subject, the statements need to be modified to use the same word (or, if they are meant to be different, the words must be defined to be so). Improved: Settle on only one term, define it in the glossary or data dictionary, and then use it consistently in each need, requirement, and design output artifact. Unacceptable: When the Input_Valve is connected to the Water_Source, the Control_Subsystem shall open the Inlet_Valve. [Two terms are used for the same thing “Input_Valve” and “Inlet_Valve”.] Improved: When the Inlet_Valve is connected to the Water_Source, the Control_Subsystem shall open the Inlet_Valve. Unacceptable: It would not be acceptable for one requirement to use one unit of measure (for example, US - feet) and another requirement to use another unit of measure (for example, Metric - meter). Guide to Writing Requirements 109 Improved: Settle on which units of measure will be used and use that unit of measure consistency across all SE artifacts including needs, Design Input Requirements and design output specifications. Also, see R40 for guidance regarding the conversion from one measurement system to another and the use of significant digits. 4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  If acronyms are used, they must be consistent throughout need and requirement sets as well as associated models and other SE artefacts developed across the lifecycle. 
-Examples:  Unacceptable: It would not be acceptable for one requirement to use the acronym “CP” for command post and another acronym “CMDP” to also refer to the “command post.” The use of two different acronyms implies that the two system elements being referred to are different. Improved: Settle on only one acronym, define it in the list of acronyms, and then use it consistently throughout the requirement set. Unacceptable: It would not be acceptable for one requirement to refer to the “Global Positioning System” and the remaining requirements refer just to “GPS.” Improved: Use the full term every time or, perhaps more usefully, define the acronym in the project acronym list or glossary and use it every time. 4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  Avoid the use of abbreviations in needs and requirement statements as well as associated models and other SE lifecycle artefacts. Guide to Writing Requirements 110 
-Examples:  Unacceptable: It would not be acceptable for one requirement to refer to the abbreviation “op” meaning operation and another to refer to the “op” meaning the operator. Improved: Avoid the abbreviation and use the full term every time. 4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  Use a project-wide style guide for individual need statements and requirement statements. 
-Examples:  For example, each organization should have a style guide or schema to address such issues as the selection and definition of what need patterns and requirement patterns should be used for writing need statements and requirement statements of a particular type, the selection and use of attributes, standard abbreviations and acronyms, layout and use of figures and tables, layout of documents or databases and, statement numbering. Guide to Writing Requirements 111 Terms used throughout the sets of needs and sets of requirements are defined in an ontology or at least a project glossary. 4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  Use a consistent format and number of signification digits for the specification of decimal numbers. 
-Examples:  Unacceptable: The &lt;SOI&gt; shall have an MTBF of less than or equal to 9.499,99 h. &amp; The &lt;SOI&gt; shall consume less than or equal to 0.99 W. [These two statements are unacceptable when included in the same set because a different format is used in the two statements.] Improved: The &lt;SOI&gt; shall have an MTBF of less than or equal to 9,499.99 h. &amp; The &lt;SOI&gt; shall consume less than or equal to 0.99 W. OR The &lt;SOI&gt; shall have an MTBF of less than or equal to 9.499,99 h. &amp; The &lt;SOI&gt; shall consume less than or equal to 0,99 W. Unacceptable: The &lt;SOI&gt; shall have an MTBF of less than or equal to 0.99 h. &amp; The &lt;SOI&gt; shall consume less than or equal to .99 W. [These two statements are unacceptable when included in the same set because a different format is used in the two statements.] Improved: The &lt;SOI&gt; shall have an MTBF of less than or equal to 9,499.99 h. &amp; The &lt;SOI&gt; shall consume less than or equal to 0.99 W. 4.14 Modularity 4</t>
-  </si>
-  <si>
-    <t>Requirement: {req}
-Criteria:  Group related needs and requirements together. 
-Examples:  Requirements may be related by: - type (for example, critical functions, enabling functions, safety, or security requirements); - scenario (for example, requirements arising from a single scenario). - interactions with other systems (for example interface requirements). - function (for example, multiple requirements defined for a function, each addressing a different performance characteristics, mode, state, condition, or trigger.) - capability (for example a needed capability may be released by a set of requirements that together result in the needed capability to be provided. -compliance (for example requirements whose purpose it is to implement a requirement in a standard or regulation. See R29 and the NRM for more guidance on organizing needs and requirements. 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requirement: {req}
-Criteria:  Conform to a defined structure or template for organizing sets of needs and requirements. 
-Examples:  For sets of needs or requirements, an outline can be defined that organizes them in categories or by type. Examples of Type/Category of needs and requirements include: • Function: Functional/Performance. • Fit: Operational: interactions with external systems - input, output, external interfaces, operational environmental, facility, ergonomic, compatibility with existing systems, logistics, users, training, installation, transportation, storage. • Quality (-ilities): reliability, availability, maintainability, accessibility, transportability, quality provisions, growth capacity. • Form: physical characteristics. • Compliance: – Standards and regulations—policy and regulatory. – Constraints—imposed on the project and the project must show compliance. – Business rules—a rule imposed by the enterprise or business unit. – Business requirements—a requirement imposed by the enterprise or business unit. Refer to the NRM Sections 4 and 6 for a more detailed discussion on this approach to organizing needs and requirements. Outlines for organizing needs and requirements can come from international standards or an organizational standard tailored to the organization’s domain and different types of products within that domain. (The organization for system level needs and requirements may be different than the organization of a set of software needs and requirements.) </t>
+Criteria:
+ Conform to a defined structure or template for organizing sets of needs and requirements. 
+Examples:
+ For sets of needs or requirements, an outline can be defined that organizes them in categories or by type. Examples of Type/Category of needs and requirements include: • Function: Functional/Performance. • Fit: Operational: interactions with external systems - input, output, external interfaces, operational environmental, facility, ergonomic, compatibility with existing systems, logistics, users, training, installation, transportation, storage. • Quality (-ilities): reliability, availability, maintainability, accessibility, transportability, quality provisions, growth capacity. • Form: physical characteristics. • Compliance: – Standards and regulations—policy and regulatory. – Constraints—imposed on the project and the project must show compliance. – Business rules—a rule imposed by the enterprise or business unit. – Business requirements—a requirement imposed by the enterprise or business unit. Refer to the NRM Sections 4 and 6 for a more detailed discussion on this approach to organizing needs and requirements. Outlines for organizing needs and requirements can come from international standards or an organizational standard tailored to the organization’s domain and different types of products within that domain. (The organization for system level needs and requirements may be different than the organization of a set of software needs and requirements.) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -961,24 +1040,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1016,7 +1104,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1050,6 +1138,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1084,9 +1173,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1259,14 +1349,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1300,14 +1392,8 @@
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1318,10 +1404,10 @@
         <v>1800</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F2">
         <v>1800</v>
@@ -1330,28 +1416,22 @@
         <v>3447</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L2" t="s">
-        <v>224</v>
-      </c>
-      <c r="M2" t="s">
-        <v>223</v>
-      </c>
-      <c r="N2" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1362,10 +1442,10 @@
         <v>3452</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3">
         <v>3452</v>
@@ -1374,28 +1454,22 @@
         <v>7150</v>
       </c>
       <c r="H3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K3" t="s">
+        <v>221</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="L3" t="s">
-        <v>224</v>
-      </c>
-      <c r="M3" t="s">
-        <v>223</v>
-      </c>
-      <c r="N3" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1406,10 +1480,10 @@
         <v>7155</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F4">
         <v>7155</v>
@@ -1418,28 +1492,22 @@
         <v>15669</v>
       </c>
       <c r="H4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="K4" t="s">
-        <v>223</v>
-      </c>
-      <c r="L4" t="s">
+        <v>221</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="M4" t="s">
-        <v>223</v>
-      </c>
-      <c r="N4" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1450,10 +1518,10 @@
         <v>15674</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F5">
         <v>15674</v>
@@ -1462,28 +1530,22 @@
         <v>19994</v>
       </c>
       <c r="H5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="I5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="J5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L5" t="s">
-        <v>224</v>
-      </c>
-      <c r="M5" t="s">
-        <v>223</v>
-      </c>
-      <c r="N5" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1494,10 +1556,10 @@
         <v>19999</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F6">
         <v>19999</v>
@@ -1506,28 +1568,22 @@
         <v>23557</v>
       </c>
       <c r="H6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="J6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L6" t="s">
-        <v>224</v>
-      </c>
-      <c r="M6" t="s">
-        <v>223</v>
-      </c>
-      <c r="N6" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1538,10 +1594,10 @@
         <v>23562</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F7">
         <v>23562</v>
@@ -1550,28 +1606,22 @@
         <v>28517</v>
       </c>
       <c r="H7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="J7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L7" t="s">
-        <v>224</v>
-      </c>
-      <c r="M7" t="s">
-        <v>223</v>
-      </c>
-      <c r="N7" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1582,10 +1632,10 @@
         <v>28522</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F8">
         <v>28522</v>
@@ -1594,28 +1644,22 @@
         <v>31796</v>
       </c>
       <c r="H8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="J8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L8" t="s">
-        <v>224</v>
-      </c>
-      <c r="M8" t="s">
-        <v>223</v>
-      </c>
-      <c r="N8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1626,10 +1670,10 @@
         <v>31801</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F9">
         <v>31801</v>
@@ -1638,28 +1682,22 @@
         <v>33551</v>
       </c>
       <c r="H9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L9" t="s">
-        <v>224</v>
-      </c>
-      <c r="M9" t="s">
-        <v>223</v>
-      </c>
-      <c r="N9" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1670,10 +1708,10 @@
         <v>33556</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F10">
         <v>33556</v>
@@ -1682,28 +1720,22 @@
         <v>36203</v>
       </c>
       <c r="H10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="K10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L10" t="s">
-        <v>224</v>
-      </c>
-      <c r="M10" t="s">
-        <v>223</v>
-      </c>
-      <c r="N10" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1714,10 +1746,10 @@
         <v>36208</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F11">
         <v>36208</v>
@@ -1726,28 +1758,22 @@
         <v>40819</v>
       </c>
       <c r="H11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="K11" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L11" t="s">
-        <v>224</v>
-      </c>
-      <c r="M11" t="s">
-        <v>223</v>
-      </c>
-      <c r="N11" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1758,10 +1784,10 @@
         <v>40824</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F12">
         <v>40824</v>
@@ -1770,28 +1796,22 @@
         <v>43155</v>
       </c>
       <c r="H12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="J12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L12" t="s">
-        <v>224</v>
-      </c>
-      <c r="M12" t="s">
-        <v>223</v>
-      </c>
-      <c r="N12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1802,10 +1822,10 @@
         <v>43160</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F13">
         <v>43160</v>
@@ -1814,28 +1834,22 @@
         <v>47520</v>
       </c>
       <c r="H13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J13" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="K13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L13" t="s">
-        <v>224</v>
-      </c>
-      <c r="M13" t="s">
-        <v>223</v>
-      </c>
-      <c r="N13" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1846,10 +1860,10 @@
         <v>47525</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F14">
         <v>47525</v>
@@ -1858,28 +1872,22 @@
         <v>50980</v>
       </c>
       <c r="H14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="I14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="K14" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L14" t="s">
-        <v>224</v>
-      </c>
-      <c r="M14" t="s">
-        <v>223</v>
-      </c>
-      <c r="N14" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1890,10 +1898,10 @@
         <v>50985</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F15">
         <v>50985</v>
@@ -1902,28 +1910,22 @@
         <v>52989</v>
       </c>
       <c r="H15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I15" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K15" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L15" t="s">
-        <v>224</v>
-      </c>
-      <c r="M15" t="s">
-        <v>223</v>
-      </c>
-      <c r="N15" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1934,10 +1936,10 @@
         <v>52994</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F16">
         <v>52994</v>
@@ -1946,28 +1948,22 @@
         <v>55944</v>
       </c>
       <c r="H16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="I16" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J16" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="K16" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L16" t="s">
-        <v>224</v>
-      </c>
-      <c r="M16" t="s">
-        <v>223</v>
-      </c>
-      <c r="N16" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1978,10 +1974,10 @@
         <v>55949</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F17">
         <v>55949</v>
@@ -1990,28 +1986,22 @@
         <v>58746</v>
       </c>
       <c r="H17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="I17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K17" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L17" t="s">
-        <v>224</v>
-      </c>
-      <c r="M17" t="s">
-        <v>223</v>
-      </c>
-      <c r="N17" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2022,10 +2012,10 @@
         <v>58751</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F18">
         <v>58751</v>
@@ -2034,28 +2024,22 @@
         <v>61364</v>
       </c>
       <c r="H18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="I18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="J18" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="K18" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L18" t="s">
-        <v>224</v>
-      </c>
-      <c r="M18" t="s">
-        <v>223</v>
-      </c>
-      <c r="N18" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2066,10 +2050,10 @@
         <v>61369</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F19">
         <v>61369</v>
@@ -2078,28 +2062,22 @@
         <v>69861</v>
       </c>
       <c r="H19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="J19" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L19" t="s">
-        <v>224</v>
-      </c>
-      <c r="M19" t="s">
-        <v>223</v>
-      </c>
-      <c r="N19" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2110,10 +2088,10 @@
         <v>69866</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F20">
         <v>69866</v>
@@ -2122,28 +2100,22 @@
         <v>72687</v>
       </c>
       <c r="H20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="I20" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J20" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K20" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L20" t="s">
-        <v>224</v>
-      </c>
-      <c r="M20" t="s">
-        <v>223</v>
-      </c>
-      <c r="N20" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2154,10 +2126,10 @@
         <v>72692</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F21">
         <v>72692</v>
@@ -2166,28 +2138,22 @@
         <v>74869</v>
       </c>
       <c r="H21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I21" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J21" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="K21" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L21" t="s">
-        <v>224</v>
-      </c>
-      <c r="M21" t="s">
-        <v>223</v>
-      </c>
-      <c r="N21" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2198,10 +2164,10 @@
         <v>74874</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F22">
         <v>74874</v>
@@ -2210,28 +2176,22 @@
         <v>77375</v>
       </c>
       <c r="H22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="I22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="K22" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L22" t="s">
-        <v>224</v>
-      </c>
-      <c r="M22" t="s">
-        <v>223</v>
-      </c>
-      <c r="N22" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2242,10 +2202,10 @@
         <v>77380</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F23">
         <v>77380</v>
@@ -2254,28 +2214,22 @@
         <v>81291</v>
       </c>
       <c r="H23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="J23" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L23" t="s">
-        <v>224</v>
-      </c>
-      <c r="M23" t="s">
-        <v>223</v>
-      </c>
-      <c r="N23" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2286,10 +2240,10 @@
         <v>81296</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F24">
         <v>81296</v>
@@ -2298,28 +2252,22 @@
         <v>85351</v>
       </c>
       <c r="H24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J24" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K24" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L24" t="s">
-        <v>224</v>
-      </c>
-      <c r="M24" t="s">
-        <v>223</v>
-      </c>
-      <c r="N24" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2330,10 +2278,10 @@
         <v>85356</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F25">
         <v>85356</v>
@@ -2342,28 +2290,22 @@
         <v>87840</v>
       </c>
       <c r="H25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="I25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="J25" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K25" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L25" t="s">
-        <v>224</v>
-      </c>
-      <c r="M25" t="s">
-        <v>223</v>
-      </c>
-      <c r="N25" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2374,10 +2316,10 @@
         <v>87845</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F26">
         <v>87845</v>
@@ -2386,28 +2328,22 @@
         <v>90144</v>
       </c>
       <c r="H26" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="I26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="J26" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L26" t="s">
-        <v>224</v>
-      </c>
-      <c r="M26" t="s">
-        <v>223</v>
-      </c>
-      <c r="N26" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2418,10 +2354,10 @@
         <v>90149</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F27">
         <v>90149</v>
@@ -2430,28 +2366,22 @@
         <v>92601</v>
       </c>
       <c r="H27" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="I27" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="J27" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L27" t="s">
-        <v>224</v>
-      </c>
-      <c r="M27" t="s">
-        <v>223</v>
-      </c>
-      <c r="N27" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2462,10 +2392,10 @@
         <v>92606</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F28">
         <v>92606</v>
@@ -2474,28 +2404,22 @@
         <v>95914</v>
       </c>
       <c r="H28" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J28" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K28" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L28" t="s">
-        <v>224</v>
-      </c>
-      <c r="M28" t="s">
-        <v>223</v>
-      </c>
-      <c r="N28" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2506,10 +2430,10 @@
         <v>95919</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E29" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F29">
         <v>95919</v>
@@ -2518,28 +2442,22 @@
         <v>99109</v>
       </c>
       <c r="H29" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I29" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J29" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L29" t="s">
-        <v>224</v>
-      </c>
-      <c r="M29" t="s">
-        <v>223</v>
-      </c>
-      <c r="N29" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2550,10 +2468,10 @@
         <v>99114</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E30" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F30">
         <v>99114</v>
@@ -2562,28 +2480,22 @@
         <v>101884</v>
       </c>
       <c r="H30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J30" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="K30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L30" t="s">
-        <v>224</v>
-      </c>
-      <c r="M30" t="s">
-        <v>223</v>
-      </c>
-      <c r="N30" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2594,10 +2506,10 @@
         <v>101889</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E31" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F31">
         <v>101889</v>
@@ -2606,28 +2518,22 @@
         <v>103395</v>
       </c>
       <c r="H31" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="I31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J31" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K31" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L31" t="s">
-        <v>224</v>
-      </c>
-      <c r="M31" t="s">
-        <v>223</v>
-      </c>
-      <c r="N31" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2638,10 +2544,10 @@
         <v>103400</v>
       </c>
       <c r="D32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F32">
         <v>103400</v>
@@ -2650,28 +2556,22 @@
         <v>112992</v>
       </c>
       <c r="H32" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I32" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="J32" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="K32" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L32" t="s">
-        <v>224</v>
-      </c>
-      <c r="M32" t="s">
-        <v>223</v>
-      </c>
-      <c r="N32" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2682,10 +2582,10 @@
         <v>112998</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F33">
         <v>112998</v>
@@ -2694,28 +2594,22 @@
         <v>114418</v>
       </c>
       <c r="H33" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="I33" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="J33" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="K33" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L33" t="s">
-        <v>224</v>
-      </c>
-      <c r="M33" t="s">
-        <v>223</v>
-      </c>
-      <c r="N33" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2726,10 +2620,10 @@
         <v>114424</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F34">
         <v>114424</v>
@@ -2738,28 +2632,22 @@
         <v>121192</v>
       </c>
       <c r="H34" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I34" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J34" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="K34" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L34" t="s">
-        <v>224</v>
-      </c>
-      <c r="M34" t="s">
-        <v>223</v>
-      </c>
-      <c r="N34" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2770,10 +2658,10 @@
         <v>121198</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E35" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F35">
         <v>121198</v>
@@ -2782,28 +2670,22 @@
         <v>123534</v>
       </c>
       <c r="H35" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I35" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="J35" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="K35" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L35" t="s">
-        <v>224</v>
-      </c>
-      <c r="M35" t="s">
-        <v>223</v>
-      </c>
-      <c r="N35" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2814,10 +2696,10 @@
         <v>123540</v>
       </c>
       <c r="D36" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F36">
         <v>123540</v>
@@ -2826,28 +2708,22 @@
         <v>124532</v>
       </c>
       <c r="H36" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I36" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J36" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="K36" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L36" t="s">
-        <v>224</v>
-      </c>
-      <c r="M36" t="s">
-        <v>223</v>
-      </c>
-      <c r="N36" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2858,10 +2734,10 @@
         <v>124538</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F37">
         <v>124538</v>
@@ -2870,28 +2746,22 @@
         <v>128633</v>
       </c>
       <c r="H37" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I37" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="J37" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K37" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L37" t="s">
-        <v>224</v>
-      </c>
-      <c r="M37" t="s">
-        <v>223</v>
-      </c>
-      <c r="N37" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2902,10 +2772,10 @@
         <v>128639</v>
       </c>
       <c r="D38" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F38">
         <v>128639</v>
@@ -2914,28 +2784,22 @@
         <v>130740</v>
       </c>
       <c r="H38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I38" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="J38" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K38" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L38" t="s">
-        <v>224</v>
-      </c>
-      <c r="M38" t="s">
-        <v>223</v>
-      </c>
-      <c r="N38" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2946,10 +2810,10 @@
         <v>130746</v>
       </c>
       <c r="D39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F39">
         <v>130746</v>
@@ -2958,28 +2822,22 @@
         <v>131784</v>
       </c>
       <c r="H39" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I39" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J39" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="K39" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L39" t="s">
-        <v>224</v>
-      </c>
-      <c r="M39" t="s">
-        <v>223</v>
-      </c>
-      <c r="N39" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2990,10 +2848,10 @@
         <v>131790</v>
       </c>
       <c r="D40" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E40" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F40">
         <v>131790</v>
@@ -3002,28 +2860,22 @@
         <v>134021</v>
       </c>
       <c r="H40" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I40" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J40" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K40" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L40" t="s">
-        <v>224</v>
-      </c>
-      <c r="M40" t="s">
-        <v>223</v>
-      </c>
-      <c r="N40" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3034,10 +2886,10 @@
         <v>134027</v>
       </c>
       <c r="D41" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E41" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F41">
         <v>134027</v>
@@ -3046,28 +2898,22 @@
         <v>138479</v>
       </c>
       <c r="H41" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I41" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J41" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="K41" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L41" t="s">
-        <v>224</v>
-      </c>
-      <c r="M41" t="s">
-        <v>223</v>
-      </c>
-      <c r="N41" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3078,10 +2924,10 @@
         <v>138485</v>
       </c>
       <c r="D42" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E42" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F42">
         <v>138485</v>
@@ -3090,28 +2936,22 @@
         <v>140419</v>
       </c>
       <c r="H42" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="I42" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="J42" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K42" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L42" t="s">
-        <v>224</v>
-      </c>
-      <c r="M42" t="s">
-        <v>223</v>
-      </c>
-      <c r="N42" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3122,10 +2962,10 @@
         <v>140425</v>
       </c>
       <c r="D43" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F43">
         <v>140425</v>
@@ -3134,25 +2974,19 @@
         <v>142847</v>
       </c>
       <c r="H43" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="I43" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="J43" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="K43" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L43" t="s">
-        <v>224</v>
-      </c>
-      <c r="M43" t="s">
-        <v>223</v>
-      </c>
-      <c r="N43" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to preprocess module, main script
</commit_message>
<xml_diff>
--- a/src/data/incose_guide_sections_df.xlsx
+++ b/src/data/incose_guide_sections_df.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d350839dcbf84db5/Desktop/github_projects/venv_aiswre/aiswre/src/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_08D160E1437B4E12A72D4C19F52F13EF797CFBCE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F24448A4-8AD5-46E0-9682-D6492A511AF2}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -367,7 +361,7 @@
     <t xml:space="preserve"> R20 – PURPOSE PHRASES Definition: Avoid phrases that indicate the “purpose of “, “intent of”, or “reason for” the need statement or requirement statement. Elaboration: Need statements and requirement statements should be as concise as possible and be Complete (C4). In an attempt to avoid ambiguity or communicate why the need or requirement is Necessary (C1), some writers include additional information to make the purpose, intent, and reason clearer by including additional text within the need statement or requirement statement or include an additional sentence of explanation immediately following the need statement or requirement statement. The text of a need statement or requirement statement should not include this extra text, nor should an additional sentence be included as part of the need or requirement statements. Expressions of purpose or intent are often indicated by the presence of phrases such as “……to”, “in order to”, “so that”, and “thus allowing.” This rule does not mean to imply that the additional information with regard to purpose is superfluous and should not be included at all. On the contrary, this extra information is useful to readers of a statement, but it should not be included in the statement; rather it should be included separately in the need expression or requirement expression using the Rationale attribute (A1) as discussed in the NRM. Examples: Unacceptable: The Record_Subsystem shall display the Name of each Line_Item so that the Operator can confirm that it is the correct Item. [This is unacceptable because the text “so that the Operator can confirm that it is the correct Item” is rationale.] Improved: The Record_Subsystem shall display the Name of each Line_Item per &lt;Display Standard XYZ&gt;. [The text “so that the Operator can confirm that it is the correct Item” should be included in the rationale attribute.] Guide to Writing Requirements 90 Unacceptable: The Operation_Logger shall record each Warning_Message produced by the system. [This is unacceptable because of the superfluous words “produced by the system”.] Improved: The Operation_Logger shall record each Warning_Message within &lt;performance measure&gt;. 4</t>
   </si>
   <si>
-    <t xml:space="preserve"> R21 – PARENTHESES Definition: Avoid parentheses and brackets containing subordinate text. Elaboration: If the text of a need statement or requirement statement contains parentheses or brackets, it usually indicates the presence of superfluous information that can simply be removed or can be communicated in the rationale. Other times, brackets introduce ambiguity. If the information in the parentheses or brackets aids in the understanding of the intent of the requirement, then that information should be included in the Rationale Attribute (A1) defined in the NRM. Conventions for the use of parentheses or brackets may be agreed upon for specific purposes. Such conventions should be documented in the project’s requirements and work instructions concerning defining needs and requirements. Examples: Unacceptable: When the Water_Temperature exceeds 85 °C (usually towards the end of the boiling cycle), the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt; [This is unacceptable because of the parenthetical phrase as well as the ambiguous word “usually”. Note that the parameter Water_Temperature needs to be defined in the glossary in order to be specific] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt;. [Note: for the above example, if this behavior is the result of a design decision, then the requirement needs to be communicated as a design output. The design input requirement should focus on why this behavior is needed - for example, prevent the boiler from over pressurizing and exploding. This is a good example of the benefit of asking “Why” for requirements of this type. The answer is the real design input requirement. If included in the set of Design Input Requirements, then the “why” should be included in the rationale.] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall prevent the Boiler from over pressurization. [How this is done is a design decision.} Exceptions and relationships: While this rule states brackets are to be avoided, R15 indicates that brackets may be used as part of a convention for eliminating ambiguous conditions such as logical expressions. In that case, it is useful to settle on a combination to be used—that is, for example, the organization Guide to Writing Requirements 91 template may avoid round brackets “( )” in any statement and may use square brackets “[...]” in logical expressions. 4</t>
+    <t xml:space="preserve"> R21 – PARENTHESES Definition: Avoid parentheses and brackets containing subordinate text. Elaboration: If the text of a need statement or requirement statement contains parentheses or brackets, it usually indicates the presence of superfluous information that can simply be removed or can be communicated in the rationale. Other times, brackets introduce ambiguity. If the information in the parentheses or brackets aids in the understanding of the intent of the requirement, then that information should be included in the Rationale Attribute (A1) defined in the NRM. Conventions for the use of parentheses or brackets may be agreed upon for specific purposes. Such conventions should be documented in the project’s requirements and work instructions concerning defining needs and requirements. Examples: Unacceptable: When the Water_Temperature exceeds 85 °C (usually towards the end of the boiling cycle), the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt; [This is unacceptable because of the parenthetical phrase as well as the ambiguous word “usually”. Note that the parameter Water_Temperature needs to be defined in the glossary in order to be specific] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt;. [Note: for the above example, if this behavior is the result of a design decision, then the requirement needs to be communicated as a design output. The design input requirement should focus on why this behavior is needed - for example, prevent the boiler from over pressurizing and exploding. This is a good example of the benefit of asking “Why” for requirements of this type. The answer is the real design input requirement. If included in the set of Design Input Requirements, then the “why” should be included in the rationale.] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall prevent the Boiler from over pressurization. [How this is done is a design decision. Exceptions and relationships: While this rule states brackets are to be avoided, R15 indicates that brackets may be used as part of a convention for eliminating ambiguous conditions such as logical expressions. In that case, it is useful to settle on a combination to be used—that is, for example, the organization Guide to Writing Requirements 91 template may avoid round brackets “( )” in any statement and may use square brackets “[...]” in logical expressions. 4</t>
   </si>
   <si>
     <t xml:space="preserve"> R22 – ENUMERATION Definition: Enumerate sets explicitly instead of using a group noun to name the set. Elaboration: If a number of functions are implied, a need statement or requirement statement should be written for each. The use of a group noun to combine functions or entities is often ambiguous because it leaves membership of that group in doubt. Other issues include allocation, traceability, verification, and validation. As with the singularity characteristic C5, each member of the set could be allocated differently, have different child requirements, each of which must be individually verified and validated. It is almost always best to list all the members of the set as separate needs or requirements. See exceptions and relationship discussion below. See also R18. Examples: Unacceptable: The thermal control system shall manage temperature-related functions. [This is unacceptable because there is ambiguity regarding which functions are to be managed as well as what is meant by “managed”. The specific functions should be enumerated explicitly in separate requirement statements along with performance expectations and any applicable conditions, triggers, or constraints.] Unacceptable: The thermal control system shall monitor system temperature. This is unacceptable because there is ambiguity regarding the function “monitor”. Similar to “managed” What are the expectations of the stakeholders – update the display of the system temperature, maintain the temperature within some range, or store the history of the system temperature? The specific subfunctions should be enumerated explicitly in separate requirement statements along with performance expectations and any applicable conditions, triggers, or constraints.] Improved: (three separate requirements): The Thermal_Control_System shall update the display of System_Temperature every 10 +/- 1 seconds. The Thermal_Control_System shall maintain the System_Temperature between 95°C and 98°C. The Thermal_Control_System shall store the history of System_Temperature. [Note use of the glossary to define terms.] Exceptions and relationships: It is almost always better to enumerate members in a set, but the rule may be softened at the higher levels of abstraction if the resulting requirement is sufficiently unambiguous. For example, at the business management level the business may state “ACME Consulting shall manage Guide to Writing Requirements 92 Human Relations (HR) functions centrally.” or a system-level need statement may state: “The &lt;stakeholders&gt; need the &lt;SOI&gt; to manage HR functions centrally.” Although this raises the question of which HR functions are being referred to, it is not useful to include a long list at these levels of abstractions and it is often not necessary since the statement is sufficiently clear at the level at which it is stated. The detailed enumeration of functions will be undertaken at the business operations level, and the business management stakeholders should be comfortable that no function will be omitted as a result of not listing it at the business management level. At the system level, need statements may include group nouns to name a set of entities or include a higher-level function that is appropriate to the level of abstraction being communicated within the need statement. During the transformation of the need statement into requirements, the project team would decompose the need into individual functional/performance requirements as well as define requirements concerning the word “centrally” and would then validate with the stakeholders that the resulting requirements, when realized, would meet the intent of the need statement. Another exemption would be to use the glossary or data dictionary to explicitly elaborate the set. For example. “Account_Information” may be defined in the Glossary to include “Account_Name”, “Account_Number”, and “Account_Balance”. 4</t>
@@ -619,7 +613,7 @@
     <t xml:space="preserve"> Unacceptable: The Record_Subsystem shall display the Name of each Line_Item so that the Operator can confirm that it is the correct Item. [This is unacceptable because the text “so that the Operator can confirm that it is the correct Item” is rationale.] Improved: The Record_Subsystem shall display the Name of each Line_Item per &lt;Display Standard XYZ&gt;. [The text “so that the Operator can confirm that it is the correct Item” should be included in the rationale attribute.] Guide to Writing Requirements 90 Unacceptable: The Operation_Logger shall record each Warning_Message produced by the system. [This is unacceptable because of the superfluous words “produced by the system”.] Improved: The Operation_Logger shall record each Warning_Message within &lt;performance measure&gt;. 4</t>
   </si>
   <si>
-    <t xml:space="preserve"> Unacceptable: When the Water_Temperature exceeds 85 °C (usually towards the end of the boiling cycle), the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt; [This is unacceptable because of the parenthetical phrase as well as the ambiguous word “usually”. Note that the parameter Water_Temperature needs to be defined in the glossary in order to be specific] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt;. [Note: for the above example, if this behavior is the result of a design decision, then the requirement needs to be communicated as a design output. The design input requirement should focus on why this behavior is needed - for example, prevent the boiler from over pressurizing and exploding. This is a good example of the benefit of asking “Why” for requirements of this type. The answer is the real design input requirement. If included in the set of Design Input Requirements, then the “why” should be included in the rationale.] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall prevent the Boiler from over pressurization. [How this is done is a design decision.} </t>
+    <t xml:space="preserve"> Unacceptable: When the Water_Temperature exceeds 85 °C (usually towards the end of the boiling cycle), the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt; [This is unacceptable because of the parenthetical phrase as well as the ambiguous word “usually”. Note that the parameter Water_Temperature needs to be defined in the glossary in order to be specific] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt;. [Note: for the above example, if this behavior is the result of a design decision, then the requirement needs to be communicated as a design output. The design input requirement should focus on why this behavior is needed - for example, prevent the boiler from over pressurizing and exploding. This is a good example of the benefit of asking “Why” for requirements of this type. The answer is the real design input requirement. If included in the set of Design Input Requirements, then the “why” should be included in the rationale.] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall prevent the Boiler from over pressurization. [How this is done is a design decision. </t>
   </si>
   <si>
     <t xml:space="preserve"> Unacceptable: The thermal control system shall manage temperature-related functions. [This is unacceptable because there is ambiguity regarding which functions are to be managed as well as what is meant by “managed”. The specific functions should be enumerated explicitly in separate requirement statements along with performance expectations and any applicable conditions, triggers, or constraints.] Unacceptable: The thermal control system shall monitor system temperature. This is unacceptable because there is ambiguity regarding the function “monitor”. Similar to “managed” What are the expectations of the stakeholders – update the display of the system temperature, maintain the temperature within some range, or store the history of the system temperature? The specific subfunctions should be enumerated explicitly in separate requirement statements along with performance expectations and any applicable conditions, triggers, or constraints.] Improved: (three separate requirements): The Thermal_Control_System shall update the display of System_Temperature every 10 +/- 1 seconds. The Thermal_Control_System shall maintain the System_Temperature between 95°C and 98°C. The Thermal_Control_System shall store the history of System_Temperature. [Note use of the glossary to define terms.] </t>
@@ -834,7 +828,7 @@
 Criteria:
  Avoid parentheses and brackets containing subordinate text. 
 Examples:
- Unacceptable: When the Water_Temperature exceeds 85 °C (usually towards the end of the boiling cycle), the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt; [This is unacceptable because of the parenthetical phrase as well as the ambiguous word “usually”. Note that the parameter Water_Temperature needs to be defined in the glossary in order to be specific] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt;. [Note: for the above example, if this behavior is the result of a design decision, then the requirement needs to be communicated as a design output. The design input requirement should focus on why this behavior is needed - for example, prevent the boiler from over pressurizing and exploding. This is a good example of the benefit of asking “Why” for requirements of this type. The answer is the real design input requirement. If included in the set of Design Input Requirements, then the “why” should be included in the rationale.] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall prevent the Boiler from over pressurization. [How this is done is a design decision.} </t>
+ Unacceptable: When the Water_Temperature exceeds 85 °C (usually towards the end of the boiling cycle), the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt; [This is unacceptable because of the parenthetical phrase as well as the ambiguous word “usually”. Note that the parameter Water_Temperature needs to be defined in the glossary in order to be specific] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall disconnect power from the Boiler within &lt;xxx ms&gt;. [Note: for the above example, if this behavior is the result of a design decision, then the requirement needs to be communicated as a design output. The design input requirement should focus on why this behavior is needed - for example, prevent the boiler from over pressurizing and exploding. This is a good example of the benefit of asking “Why” for requirements of this type. The answer is the real design input requirement. If included in the set of Design Input Requirements, then the “why” should be included in the rationale.] Improved: If the Water_Temperature increases to greater than 85 °C, the Control_Unit shall prevent the Boiler from over pressurization. [How this is done is a design decision. </t>
   </si>
   <si>
     <t xml:space="preserve">Requirement: {req}
@@ -987,8 +981,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1040,33 +1034,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1104,7 +1089,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1138,7 +1123,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1173,10 +1157,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1349,16 +1332,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1393,7 +1374,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1431,7 +1412,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1465,11 +1446,11 @@
       <c r="K3" t="s">
         <v>221</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1503,11 +1484,11 @@
       <c r="K4" t="s">
         <v>221</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1545,7 +1526,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1583,7 +1564,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1621,7 +1602,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1659,7 +1640,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1697,7 +1678,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1735,7 +1716,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1773,7 +1754,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1811,7 +1792,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1849,7 +1830,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1887,7 +1868,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1925,7 +1906,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1963,7 +1944,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2001,7 +1982,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2039,7 +2020,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2077,7 +2058,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2115,7 +2096,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2153,7 +2134,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2173,7 +2154,7 @@
         <v>74874</v>
       </c>
       <c r="G22">
-        <v>77375</v>
+        <v>77374</v>
       </c>
       <c r="H22" t="s">
         <v>115</v>
@@ -2191,15 +2172,15 @@
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>77375</v>
+        <v>77374</v>
       </c>
       <c r="C23">
-        <v>77380</v>
+        <v>77379</v>
       </c>
       <c r="D23" t="s">
         <v>32</v>
@@ -2208,10 +2189,10 @@
         <v>74</v>
       </c>
       <c r="F23">
-        <v>77380</v>
+        <v>77379</v>
       </c>
       <c r="G23">
-        <v>81291</v>
+        <v>81290</v>
       </c>
       <c r="H23" t="s">
         <v>116</v>
@@ -2229,15 +2210,15 @@
         <v>243</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>81291</v>
+        <v>81290</v>
       </c>
       <c r="C24">
-        <v>81296</v>
+        <v>81295</v>
       </c>
       <c r="D24" t="s">
         <v>33</v>
@@ -2246,10 +2227,10 @@
         <v>75</v>
       </c>
       <c r="F24">
-        <v>81296</v>
+        <v>81295</v>
       </c>
       <c r="G24">
-        <v>85351</v>
+        <v>85350</v>
       </c>
       <c r="H24" t="s">
         <v>117</v>
@@ -2267,15 +2248,15 @@
         <v>244</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>85351</v>
+        <v>85350</v>
       </c>
       <c r="C25">
-        <v>85356</v>
+        <v>85355</v>
       </c>
       <c r="D25" t="s">
         <v>34</v>
@@ -2284,10 +2265,10 @@
         <v>76</v>
       </c>
       <c r="F25">
-        <v>85356</v>
+        <v>85355</v>
       </c>
       <c r="G25">
-        <v>87840</v>
+        <v>87839</v>
       </c>
       <c r="H25" t="s">
         <v>118</v>
@@ -2305,15 +2286,15 @@
         <v>245</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>87840</v>
+        <v>87839</v>
       </c>
       <c r="C26">
-        <v>87845</v>
+        <v>87844</v>
       </c>
       <c r="D26" t="s">
         <v>35</v>
@@ -2322,10 +2303,10 @@
         <v>77</v>
       </c>
       <c r="F26">
-        <v>87845</v>
+        <v>87844</v>
       </c>
       <c r="G26">
-        <v>90144</v>
+        <v>90143</v>
       </c>
       <c r="H26" t="s">
         <v>119</v>
@@ -2343,15 +2324,15 @@
         <v>246</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>90144</v>
+        <v>90143</v>
       </c>
       <c r="C27">
-        <v>90149</v>
+        <v>90148</v>
       </c>
       <c r="D27" t="s">
         <v>36</v>
@@ -2360,10 +2341,10 @@
         <v>78</v>
       </c>
       <c r="F27">
-        <v>90149</v>
+        <v>90148</v>
       </c>
       <c r="G27">
-        <v>92601</v>
+        <v>92600</v>
       </c>
       <c r="H27" t="s">
         <v>120</v>
@@ -2381,15 +2362,15 @@
         <v>247</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28">
-        <v>92601</v>
+        <v>92600</v>
       </c>
       <c r="C28">
-        <v>92606</v>
+        <v>92605</v>
       </c>
       <c r="D28" t="s">
         <v>37</v>
@@ -2398,10 +2379,10 @@
         <v>79</v>
       </c>
       <c r="F28">
-        <v>92606</v>
+        <v>92605</v>
       </c>
       <c r="G28">
-        <v>95914</v>
+        <v>95913</v>
       </c>
       <c r="H28" t="s">
         <v>121</v>
@@ -2419,15 +2400,15 @@
         <v>248</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29">
-        <v>95914</v>
+        <v>95913</v>
       </c>
       <c r="C29">
-        <v>95919</v>
+        <v>95918</v>
       </c>
       <c r="D29" t="s">
         <v>38</v>
@@ -2436,10 +2417,10 @@
         <v>80</v>
       </c>
       <c r="F29">
-        <v>95919</v>
+        <v>95918</v>
       </c>
       <c r="G29">
-        <v>99109</v>
+        <v>99108</v>
       </c>
       <c r="H29" t="s">
         <v>122</v>
@@ -2457,15 +2438,15 @@
         <v>249</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>99109</v>
+        <v>99108</v>
       </c>
       <c r="C30">
-        <v>99114</v>
+        <v>99113</v>
       </c>
       <c r="D30" t="s">
         <v>39</v>
@@ -2474,10 +2455,10 @@
         <v>81</v>
       </c>
       <c r="F30">
-        <v>99114</v>
+        <v>99113</v>
       </c>
       <c r="G30">
-        <v>101884</v>
+        <v>101883</v>
       </c>
       <c r="H30" t="s">
         <v>123</v>
@@ -2495,15 +2476,15 @@
         <v>250</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31">
-        <v>101884</v>
+        <v>101883</v>
       </c>
       <c r="C31">
-        <v>101889</v>
+        <v>101888</v>
       </c>
       <c r="D31" t="s">
         <v>40</v>
@@ -2512,10 +2493,10 @@
         <v>82</v>
       </c>
       <c r="F31">
-        <v>101889</v>
+        <v>101888</v>
       </c>
       <c r="G31">
-        <v>103395</v>
+        <v>103394</v>
       </c>
       <c r="H31" t="s">
         <v>124</v>
@@ -2533,15 +2514,15 @@
         <v>251</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32">
-        <v>103395</v>
+        <v>103394</v>
       </c>
       <c r="C32">
-        <v>103400</v>
+        <v>103399</v>
       </c>
       <c r="D32" t="s">
         <v>41</v>
@@ -2550,10 +2531,10 @@
         <v>83</v>
       </c>
       <c r="F32">
-        <v>103400</v>
+        <v>103399</v>
       </c>
       <c r="G32">
-        <v>112992</v>
+        <v>112991</v>
       </c>
       <c r="H32" t="s">
         <v>125</v>
@@ -2571,15 +2552,15 @@
         <v>252</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33">
-        <v>112992</v>
+        <v>112991</v>
       </c>
       <c r="C33">
-        <v>112998</v>
+        <v>112997</v>
       </c>
       <c r="D33" t="s">
         <v>42</v>
@@ -2588,10 +2569,10 @@
         <v>84</v>
       </c>
       <c r="F33">
-        <v>112998</v>
+        <v>112997</v>
       </c>
       <c r="G33">
-        <v>114418</v>
+        <v>114417</v>
       </c>
       <c r="H33" t="s">
         <v>126</v>
@@ -2609,15 +2590,15 @@
         <v>253</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34">
-        <v>114418</v>
+        <v>114417</v>
       </c>
       <c r="C34">
-        <v>114424</v>
+        <v>114423</v>
       </c>
       <c r="D34" t="s">
         <v>43</v>
@@ -2626,10 +2607,10 @@
         <v>85</v>
       </c>
       <c r="F34">
-        <v>114424</v>
+        <v>114423</v>
       </c>
       <c r="G34">
-        <v>121192</v>
+        <v>121191</v>
       </c>
       <c r="H34" t="s">
         <v>127</v>
@@ -2647,15 +2628,15 @@
         <v>254</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35">
-        <v>121192</v>
+        <v>121191</v>
       </c>
       <c r="C35">
-        <v>121198</v>
+        <v>121197</v>
       </c>
       <c r="D35" t="s">
         <v>44</v>
@@ -2664,10 +2645,10 @@
         <v>86</v>
       </c>
       <c r="F35">
-        <v>121198</v>
+        <v>121197</v>
       </c>
       <c r="G35">
-        <v>123534</v>
+        <v>123533</v>
       </c>
       <c r="H35" t="s">
         <v>128</v>
@@ -2685,15 +2666,15 @@
         <v>255</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36">
-        <v>123534</v>
+        <v>123533</v>
       </c>
       <c r="C36">
-        <v>123540</v>
+        <v>123539</v>
       </c>
       <c r="D36" t="s">
         <v>45</v>
@@ -2702,10 +2683,10 @@
         <v>87</v>
       </c>
       <c r="F36">
-        <v>123540</v>
+        <v>123539</v>
       </c>
       <c r="G36">
-        <v>124532</v>
+        <v>124531</v>
       </c>
       <c r="H36" t="s">
         <v>129</v>
@@ -2723,15 +2704,15 @@
         <v>256</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37">
-        <v>124532</v>
+        <v>124531</v>
       </c>
       <c r="C37">
-        <v>124538</v>
+        <v>124537</v>
       </c>
       <c r="D37" t="s">
         <v>46</v>
@@ -2740,10 +2721,10 @@
         <v>88</v>
       </c>
       <c r="F37">
-        <v>124538</v>
+        <v>124537</v>
       </c>
       <c r="G37">
-        <v>128633</v>
+        <v>128632</v>
       </c>
       <c r="H37" t="s">
         <v>130</v>
@@ -2761,15 +2742,15 @@
         <v>257</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38">
-        <v>128633</v>
+        <v>128632</v>
       </c>
       <c r="C38">
-        <v>128639</v>
+        <v>128638</v>
       </c>
       <c r="D38" t="s">
         <v>47</v>
@@ -2778,10 +2759,10 @@
         <v>89</v>
       </c>
       <c r="F38">
-        <v>128639</v>
+        <v>128638</v>
       </c>
       <c r="G38">
-        <v>130740</v>
+        <v>130739</v>
       </c>
       <c r="H38" t="s">
         <v>131</v>
@@ -2799,15 +2780,15 @@
         <v>258</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39">
-        <v>130740</v>
+        <v>130739</v>
       </c>
       <c r="C39">
-        <v>130746</v>
+        <v>130745</v>
       </c>
       <c r="D39" t="s">
         <v>48</v>
@@ -2816,10 +2797,10 @@
         <v>90</v>
       </c>
       <c r="F39">
-        <v>130746</v>
+        <v>130745</v>
       </c>
       <c r="G39">
-        <v>131784</v>
+        <v>131783</v>
       </c>
       <c r="H39" t="s">
         <v>132</v>
@@ -2837,15 +2818,15 @@
         <v>259</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40">
-        <v>131784</v>
+        <v>131783</v>
       </c>
       <c r="C40">
-        <v>131790</v>
+        <v>131789</v>
       </c>
       <c r="D40" t="s">
         <v>49</v>
@@ -2854,10 +2835,10 @@
         <v>91</v>
       </c>
       <c r="F40">
-        <v>131790</v>
+        <v>131789</v>
       </c>
       <c r="G40">
-        <v>134021</v>
+        <v>134020</v>
       </c>
       <c r="H40" t="s">
         <v>133</v>
@@ -2875,15 +2856,15 @@
         <v>260</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41">
-        <v>134021</v>
+        <v>134020</v>
       </c>
       <c r="C41">
-        <v>134027</v>
+        <v>134026</v>
       </c>
       <c r="D41" t="s">
         <v>50</v>
@@ -2892,10 +2873,10 @@
         <v>92</v>
       </c>
       <c r="F41">
-        <v>134027</v>
+        <v>134026</v>
       </c>
       <c r="G41">
-        <v>138479</v>
+        <v>138478</v>
       </c>
       <c r="H41" t="s">
         <v>134</v>
@@ -2913,15 +2894,15 @@
         <v>261</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42">
-        <v>138479</v>
+        <v>138478</v>
       </c>
       <c r="C42">
-        <v>138485</v>
+        <v>138484</v>
       </c>
       <c r="D42" t="s">
         <v>51</v>
@@ -2930,10 +2911,10 @@
         <v>93</v>
       </c>
       <c r="F42">
-        <v>138485</v>
+        <v>138484</v>
       </c>
       <c r="G42">
-        <v>140419</v>
+        <v>140418</v>
       </c>
       <c r="H42" t="s">
         <v>135</v>
@@ -2951,15 +2932,15 @@
         <v>262</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43">
-        <v>140419</v>
+        <v>140418</v>
       </c>
       <c r="C43">
-        <v>140425</v>
+        <v>140424</v>
       </c>
       <c r="D43" t="s">
         <v>52</v>
@@ -2968,10 +2949,10 @@
         <v>94</v>
       </c>
       <c r="F43">
-        <v>140425</v>
+        <v>140424</v>
       </c>
       <c r="G43">
-        <v>142847</v>
+        <v>142846</v>
       </c>
       <c r="H43" t="s">
         <v>136</v>

</xml_diff>